<commit_message>
Fix a bug in creature factory - sprint backlog updated
</commit_message>
<xml_diff>
--- a/process/Project Backlog.xlsx
+++ b/process/Project Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardoperugini/Desktop/PPS-19-Primer/process/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D08B4E-BD7E-4F43-A5AF-63CEBF47C282}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9A2FA4-3DFE-D542-8107-A1FE8C405140}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" activeTab="1" xr2:uid="{FED3A4F8-C6A4-7E4A-8252-7547BCB55159}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>Priority</t>
   </si>
@@ -452,6 +452,78 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -464,16 +536,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -481,81 +556,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -886,12 +886,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -899,233 +899,233 @@
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="11"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="35"/>
     </row>
     <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="13">
         <v>1</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="13">
         <v>2</v>
       </c>
-      <c r="H5" s="29">
-        <v>3</v>
-      </c>
-      <c r="I5" s="29">
+      <c r="H5" s="13">
+        <v>3</v>
+      </c>
+      <c r="I5" s="13">
         <v>4</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="14">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="16">
+      <c r="B6" s="37">
         <v>1</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="37">
         <v>5</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="22"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="19" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="23"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="39"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="24">
+      <c r="B8" s="10">
         <v>2</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="32" t="s">
+      <c r="D8" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="24">
-        <v>3</v>
-      </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="32"/>
+      <c r="E8" s="10">
+        <v>3</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="24">
-        <v>3</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="33" t="s">
+      <c r="B9" s="10">
+        <v>3</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="10">
         <v>4</v>
       </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="13">
+      <c r="B10" s="26">
         <v>4</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="30" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="28">
         <v>7</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="26"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="27"/>
       <c r="D11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="24">
+      <c r="B12" s="10">
         <v>5</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="10">
         <v>20</v>
       </c>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="13">
+      <c r="B13" s="26">
         <v>6</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="30" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="28">
         <v>15</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="15"/>
-      <c r="C14" s="26"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="13">
+      <c r="B15" s="26">
         <v>7</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="26">
         <v>8</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="15"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="19" t="s">
+      <c r="B16" s="27"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="24">
+      <c r="B17" s="10">
         <v>8</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -1134,57 +1134,33 @@
       <c r="E17" s="6">
         <v>11</v>
       </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="24">
+      <c r="B18" s="10">
         <v>9</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="10">
         <v>30</v>
       </c>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="F10:F11"/>
     <mergeCell ref="F4:J4"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B6:B7"/>
@@ -1195,6 +1171,30 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="E6:E7"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="F15:F16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1204,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D958F6-BD44-1941-9C2E-56BB7B285D1F}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1217,12 +1217,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
     </row>
     <row r="4" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
@@ -1235,14 +1235,14 @@
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="18"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="43"/>
     </row>
     <row r="6" spans="1:11" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -1277,348 +1277,384 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="D7" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="15">
         <v>7</v>
       </c>
-      <c r="F7" s="39">
+      <c r="F7" s="21">
         <v>1</v>
       </c>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-      <c r="K7" s="40"/>
+      <c r="G7" s="21">
+        <v>1</v>
+      </c>
+      <c r="H7" s="21"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B8" s="14"/>
-      <c r="C8" s="41" t="s">
+      <c r="B8" s="32"/>
+      <c r="C8" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="42">
-        <v>3</v>
-      </c>
-      <c r="F8" s="42">
+      <c r="E8" s="24">
+        <v>3</v>
+      </c>
+      <c r="F8" s="24">
         <v>1</v>
       </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
+      <c r="G8" s="24">
+        <v>1</v>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B9" s="14"/>
-      <c r="C9" s="41" t="s">
+      <c r="B9" s="32"/>
+      <c r="C9" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="42">
-        <v>3</v>
-      </c>
-      <c r="F9" s="42">
+      <c r="E9" s="24">
+        <v>3</v>
+      </c>
+      <c r="F9" s="24">
         <v>1</v>
       </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
+      <c r="G9" s="24">
+        <v>1</v>
+      </c>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="14"/>
-      <c r="C10" s="32" t="s">
+      <c r="B10" s="32"/>
+      <c r="C10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E10" s="42">
+      <c r="E10" s="24">
         <v>7</v>
       </c>
-      <c r="F10" s="42">
+      <c r="F10" s="24">
         <v>1</v>
       </c>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
+      <c r="G10" s="24">
+        <v>1</v>
+      </c>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B11" s="14"/>
-      <c r="C11" s="43" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E11" s="42">
+      <c r="E11" s="24">
         <v>7</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="24">
         <v>1</v>
       </c>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
+      <c r="G11" s="24">
+        <v>1</v>
+      </c>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="42" t="s">
+      <c r="D12" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="10">
         <v>15</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="24">
         <v>12</v>
       </c>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
+      <c r="G12" s="24">
+        <v>10</v>
+      </c>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C13" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="42" t="s">
+      <c r="D13" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="10">
         <v>2</v>
       </c>
-      <c r="F13" s="42">
+      <c r="F13" s="24">
         <v>0</v>
       </c>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
+      <c r="G13" s="24">
+        <v>0</v>
+      </c>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B14" s="14"/>
-      <c r="C14" s="32" t="s">
+      <c r="B14" s="32"/>
+      <c r="C14" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="42" t="s">
+      <c r="D14" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="24">
-        <v>3</v>
-      </c>
-      <c r="F14" s="42">
+      <c r="E14" s="10">
+        <v>3</v>
+      </c>
+      <c r="F14" s="24">
         <v>0</v>
       </c>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
+      <c r="G14" s="24">
+        <v>0</v>
+      </c>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B15" s="14"/>
-      <c r="C15" s="32" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="10">
         <v>2</v>
       </c>
-      <c r="F15" s="42">
+      <c r="F15" s="24">
         <v>0</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
+      <c r="G15" s="24">
+        <v>0</v>
+      </c>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B16" s="14"/>
-      <c r="C16" s="32" t="s">
+      <c r="B16" s="32"/>
+      <c r="C16" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="10">
         <v>2</v>
       </c>
-      <c r="F16" s="42">
+      <c r="F16" s="24">
         <v>0</v>
       </c>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
+      <c r="G16" s="24">
+        <v>0</v>
+      </c>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B17" s="15"/>
-      <c r="C17" s="43" t="s">
+      <c r="B17" s="27"/>
+      <c r="C17" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="10">
         <v>2</v>
       </c>
-      <c r="F17" s="42">
+      <c r="F17" s="24">
         <v>0</v>
       </c>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
+      <c r="G17" s="24">
+        <v>0</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="32" t="s">
+      <c r="B18" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24">
-        <v>3</v>
-      </c>
-      <c r="F18" s="42">
-        <v>3</v>
-      </c>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10">
+        <v>3</v>
+      </c>
+      <c r="F18" s="24">
+        <v>3</v>
+      </c>
+      <c r="G18" s="24">
+        <v>3</v>
+      </c>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="14"/>
-      <c r="C19" s="32" t="s">
+      <c r="B19" s="32"/>
+      <c r="C19" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24">
-        <v>3</v>
-      </c>
-      <c r="F19" s="42">
-        <v>3</v>
-      </c>
-      <c r="G19" s="42"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10">
+        <v>3</v>
+      </c>
+      <c r="F19" s="24">
+        <v>3</v>
+      </c>
+      <c r="G19" s="24">
+        <v>3</v>
+      </c>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="10">
         <v>4</v>
       </c>
-      <c r="F20" s="42">
+      <c r="F20" s="24">
         <v>2</v>
       </c>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
+      <c r="G20" s="24">
+        <v>2</v>
+      </c>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="14"/>
-      <c r="C21" s="32" t="s">
+      <c r="B21" s="32"/>
+      <c r="C21" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="10">
         <v>5</v>
       </c>
-      <c r="F21" s="42">
-        <v>3</v>
-      </c>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
+      <c r="F21" s="24">
+        <v>3</v>
+      </c>
+      <c r="G21" s="24">
+        <v>1</v>
+      </c>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="14"/>
-      <c r="C22" s="32" t="s">
+      <c r="B22" s="32"/>
+      <c r="C22" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="24" t="s">
+      <c r="D22" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22" s="10">
         <v>5</v>
       </c>
-      <c r="F22" s="42">
-        <v>3</v>
-      </c>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
+      <c r="F22" s="24">
+        <v>3</v>
+      </c>
+      <c r="G22" s="24">
+        <v>1</v>
+      </c>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="15"/>
-      <c r="C23" s="32" t="s">
+      <c r="B23" s="27"/>
+      <c r="C23" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24">
+      <c r="D23" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="10">
         <v>5</v>
       </c>
-      <c r="F23" s="42">
+      <c r="F23" s="24">
         <v>4</v>
       </c>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
+      <c r="G23" s="24">
+        <v>3</v>
+      </c>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
end of sprint #2 - backlog updated
</commit_message>
<xml_diff>
--- a/process/Project Backlog.xlsx
+++ b/process/Project Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardoperugini/Desktop/PPS-19-Primer/process/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E20453-A475-7E41-9907-7CC53FD93B77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49CB7E2-7468-7849-B1C0-C2CA3E1C9E71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13020" yWindow="460" windowWidth="15780" windowHeight="16760" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Riepilogo di esportazione" sheetId="1" r:id="rId1"/>
@@ -290,7 +290,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -300,18 +300,27 @@
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="12"/>
       <color indexed="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -592,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -632,9 +641,6 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -679,14 +685,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -713,7 +740,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -725,6 +752,9 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -738,10 +768,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1917,11 +1947,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
+      <c r="B3" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
     </row>
     <row r="7" spans="2:4" ht="19" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -1999,7 +2029,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2013,12 +2045,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2056,13 +2088,13 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="43" t="s">
+      <c r="F4" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="45"/>
+      <c r="G4" s="50"/>
+      <c r="H4" s="50"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="51"/>
     </row>
     <row r="5" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
@@ -2105,74 +2137,80 @@
       <c r="D6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="37">
         <v>20</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="37">
         <v>20</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
+      <c r="G6" s="38">
+        <v>5</v>
+      </c>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
-      <c r="B7" s="18">
+      <c r="B7" s="17">
         <v>2</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="39">
         <v>7</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="39">
         <v>7</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
+      <c r="G7" s="40">
+        <v>1</v>
+      </c>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
     </row>
     <row r="8" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
-      <c r="B8" s="40">
+      <c r="B8" s="46">
         <v>3</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="45">
         <v>8</v>
       </c>
-      <c r="F8" s="40">
+      <c r="F8" s="45">
         <v>8</v>
       </c>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
-      <c r="J8" s="38"/>
+      <c r="G8" s="43">
+        <v>1</v>
+      </c>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
     </row>
     <row r="9" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="22" t="s">
+      <c r="B9" s="47"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
     </row>
     <row r="10" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
@@ -2185,52 +2223,56 @@
       <c r="D10" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="37">
         <v>11</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="37">
         <v>11</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
+      <c r="G10" s="38">
+        <v>2</v>
+      </c>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
     </row>
     <row r="11" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
-      <c r="B11" s="40">
+      <c r="B11" s="46">
         <v>5</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="45">
         <v>15</v>
       </c>
-      <c r="F11" s="40">
+      <c r="F11" s="45">
         <v>15</v>
       </c>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+      <c r="G11" s="43">
+        <v>0</v>
+      </c>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
     </row>
     <row r="12" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="22" t="s">
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
     </row>
     <row r="13" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
@@ -2243,176 +2285,190 @@
       <c r="D13" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="37">
         <v>30</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="37">
         <v>25</v>
       </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
+      <c r="G13" s="38">
+        <v>20</v>
+      </c>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
-      <c r="B14" s="40">
+      <c r="B14" s="46">
         <v>7</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="40">
+      <c r="E14" s="45">
         <v>7</v>
       </c>
-      <c r="F14" s="40">
+      <c r="F14" s="45">
         <v>2</v>
       </c>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
+      <c r="G14" s="43">
+        <v>1</v>
+      </c>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
     </row>
     <row r="15" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="22" t="s">
+      <c r="B15" s="47"/>
+      <c r="C15" s="47"/>
+      <c r="D15" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
     </row>
     <row r="16" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
-      <c r="B16" s="18">
+      <c r="B16" s="17">
         <v>8</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="39">
         <v>10</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="39">
         <v>10</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
+      <c r="G16" s="40">
+        <v>3</v>
+      </c>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
-      <c r="B17" s="18">
+      <c r="B17" s="17">
         <v>9</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="D17" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="39">
         <v>17</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="39">
         <v>17</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
+      <c r="G17" s="40">
+        <v>17</v>
+      </c>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
-      <c r="B18" s="18">
+      <c r="B18" s="17">
         <v>10</v>
       </c>
       <c r="C18" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="39">
         <v>5</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="39">
         <v>5</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
+      <c r="G18" s="40">
+        <v>5</v>
+      </c>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
-      <c r="B19" s="18">
+      <c r="B19" s="17">
         <v>11</v>
       </c>
       <c r="C19" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="39">
         <v>5</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="39">
         <v>5</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
+      <c r="G19" s="40">
+        <v>5</v>
+      </c>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
-      <c r="B20" s="49">
+      <c r="B20" s="55">
         <v>12</v>
       </c>
-      <c r="C20" s="51" t="s">
+      <c r="C20" s="57" t="s">
         <v>37</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="49">
+      <c r="E20" s="58">
         <v>5</v>
       </c>
-      <c r="F20" s="49">
-        <v>0</v>
-      </c>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
+      <c r="F20" s="58">
+        <v>0</v>
+      </c>
+      <c r="G20" s="54">
+        <v>0</v>
+      </c>
+      <c r="H20" s="54"/>
+      <c r="I20" s="54"/>
+      <c r="J20" s="54"/>
     </row>
     <row r="21" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="50"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="56"/>
       <c r="D21" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="54"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
     </row>
     <row r="22" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
@@ -2425,16 +2481,18 @@
       <c r="D22" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="15">
+      <c r="E22" s="37">
         <v>3</v>
       </c>
-      <c r="F22" s="15">
-        <v>0</v>
-      </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
+      <c r="F22" s="37">
+        <v>0</v>
+      </c>
+      <c r="G22" s="38">
+        <v>0</v>
+      </c>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
     </row>
     <row r="23" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
@@ -2447,16 +2505,18 @@
       <c r="D23" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="15">
+      <c r="E23" s="37">
         <v>4</v>
       </c>
-      <c r="F23" s="15">
-        <v>0</v>
-      </c>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
+      <c r="F23" s="37">
+        <v>0</v>
+      </c>
+      <c r="G23" s="38">
+        <v>0</v>
+      </c>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="34">
@@ -2507,26 +2567,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="24" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" style="24" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" style="24" customWidth="1"/>
-    <col min="6" max="12" width="10.83203125" style="24" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="24"/>
+    <col min="1" max="1" width="10.83203125" style="23" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" style="23" customWidth="1"/>
+    <col min="6" max="12" width="10.83203125" style="23" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2579,86 +2641,86 @@
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="43" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="53"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="60"/>
     </row>
     <row r="6" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="26">
         <v>1</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="26">
         <v>2</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="26">
         <v>3</v>
       </c>
-      <c r="I6" s="27">
+      <c r="I6" s="26">
         <v>4</v>
       </c>
-      <c r="J6" s="27">
+      <c r="J6" s="26">
         <v>5</v>
       </c>
-      <c r="K6" s="27">
+      <c r="K6" s="26">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="30">
+      <c r="E7" s="29">
         <v>7</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="29">
         <v>1</v>
       </c>
-      <c r="G7" s="30">
+      <c r="G7" s="29">
         <v>1</v>
       </c>
-      <c r="H7" s="30">
-        <v>0</v>
-      </c>
-      <c r="I7" s="30">
-        <v>0</v>
-      </c>
-      <c r="J7" s="30">
-        <v>0</v>
-      </c>
-      <c r="K7" s="30">
+      <c r="H7" s="29">
+        <v>0</v>
+      </c>
+      <c r="I7" s="29">
+        <v>0</v>
+      </c>
+      <c r="J7" s="29">
+        <v>0</v>
+      </c>
+      <c r="K7" s="29">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="14"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="31" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="30" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="16" t="s">
@@ -2688,8 +2750,8 @@
     </row>
     <row r="9" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="31" t="s">
+      <c r="B9" s="61"/>
+      <c r="C9" s="30" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="16" t="s">
@@ -2719,8 +2781,8 @@
     </row>
     <row r="10" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="31" t="s">
+      <c r="B10" s="61"/>
+      <c r="C10" s="30" t="s">
         <v>54</v>
       </c>
       <c r="D10" s="16" t="s">
@@ -2750,8 +2812,8 @@
     </row>
     <row r="11" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="31" t="s">
+      <c r="B11" s="47"/>
+      <c r="C11" s="30" t="s">
         <v>55</v>
       </c>
       <c r="D11" s="16" t="s">
@@ -2784,7 +2846,7 @@
       <c r="B12" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="30" t="s">
         <v>56</v>
       </c>
       <c r="D12" s="16" t="s">
@@ -2814,10 +2876,10 @@
     </row>
     <row r="13" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="30" t="s">
         <v>57</v>
       </c>
       <c r="D13" s="16" t="s">
@@ -2847,8 +2909,8 @@
     </row>
     <row r="14" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="31" t="s">
+      <c r="B14" s="61"/>
+      <c r="C14" s="30" t="s">
         <v>58</v>
       </c>
       <c r="D14" s="16" t="s">
@@ -2878,8 +2940,8 @@
     </row>
     <row r="15" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="31" t="s">
+      <c r="B15" s="61"/>
+      <c r="C15" s="30" t="s">
         <v>59</v>
       </c>
       <c r="D15" s="16" t="s">
@@ -2909,8 +2971,8 @@
     </row>
     <row r="16" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="31" t="s">
+      <c r="B16" s="61"/>
+      <c r="C16" s="30" t="s">
         <v>60</v>
       </c>
       <c r="D16" s="16" t="s">
@@ -2940,8 +3002,8 @@
     </row>
     <row r="17" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="31" t="s">
+      <c r="B17" s="47"/>
+      <c r="C17" s="30" t="s">
         <v>61</v>
       </c>
       <c r="D17" s="16" t="s">
@@ -2971,10 +3033,10 @@
     </row>
     <row r="18" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="31" t="s">
+      <c r="C18" s="30" t="s">
         <v>62</v>
       </c>
       <c r="D18" s="16" t="s">
@@ -3004,8 +3066,8 @@
     </row>
     <row r="19" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="31" t="s">
+      <c r="B19" s="47"/>
+      <c r="C19" s="30" t="s">
         <v>63</v>
       </c>
       <c r="D19" s="16" t="s">
@@ -3035,10 +3097,10 @@
     </row>
     <row r="20" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="30" t="s">
         <v>64</v>
       </c>
       <c r="D20" s="16" t="s">
@@ -3068,8 +3130,8 @@
     </row>
     <row r="21" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="31" t="s">
+      <c r="B21" s="61"/>
+      <c r="C21" s="30" t="s">
         <v>65</v>
       </c>
       <c r="D21" s="16" t="s">
@@ -3099,8 +3161,8 @@
     </row>
     <row r="22" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="31" t="s">
+      <c r="B22" s="61"/>
+      <c r="C22" s="30" t="s">
         <v>67</v>
       </c>
       <c r="D22" s="16" t="s">
@@ -3130,8 +3192,8 @@
     </row>
     <row r="23" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
-      <c r="B23" s="41"/>
-      <c r="C23" s="31" t="s">
+      <c r="B23" s="47"/>
+      <c r="C23" s="30" t="s">
         <v>69</v>
       </c>
       <c r="D23" s="16" t="s">
@@ -3180,28 +3242,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:H18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="32" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="32" customWidth="1"/>
-    <col min="3" max="3" width="63.1640625" style="32" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="32" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" style="32" customWidth="1"/>
-    <col min="6" max="13" width="10.83203125" style="32" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="32"/>
+    <col min="1" max="1" width="10.83203125" style="31" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="31" customWidth="1"/>
+    <col min="3" max="3" width="63.1640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="31" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" style="31" customWidth="1"/>
+    <col min="6" max="13" width="10.83203125" style="31" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -3286,155 +3348,161 @@
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="43" t="s">
+      <c r="E7" s="24"/>
+      <c r="F7" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="52"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="52"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="52"/>
-      <c r="L7" s="53"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="60"/>
     </row>
     <row r="8" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="26">
         <v>1</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="26">
         <v>2</v>
       </c>
-      <c r="H8" s="27">
+      <c r="H8" s="26">
         <v>3</v>
       </c>
-      <c r="I8" s="27">
+      <c r="I8" s="26">
         <v>4</v>
       </c>
-      <c r="J8" s="27">
+      <c r="J8" s="26">
         <v>5</v>
       </c>
-      <c r="K8" s="27">
+      <c r="K8" s="26">
         <v>6</v>
       </c>
-      <c r="L8" s="27">
+      <c r="L8" s="26">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="62" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="29" t="s">
+      <c r="D9" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="33">
         <v>5</v>
       </c>
-      <c r="F9" s="34">
+      <c r="F9" s="33">
         <v>3</v>
       </c>
-      <c r="G9" s="35">
+      <c r="G9" s="34">
         <v>2</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="34">
         <v>1</v>
       </c>
-      <c r="I9" s="35">
+      <c r="I9" s="34">
         <v>1</v>
       </c>
-      <c r="J9" s="35">
+      <c r="J9" s="34">
         <v>1</v>
       </c>
-      <c r="K9" s="35">
-        <v>0</v>
-      </c>
-      <c r="L9" s="35"/>
+      <c r="K9" s="34">
+        <v>0</v>
+      </c>
+      <c r="L9" s="35">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="19" t="s">
+      <c r="B10" s="61"/>
+      <c r="C10" s="18" t="s">
         <v>73</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="17">
         <v>10</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <v>6</v>
       </c>
-      <c r="G10" s="20">
+      <c r="G10" s="19">
         <v>3</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="19">
         <v>1</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="19">
         <v>1</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="19">
         <v>1</v>
       </c>
-      <c r="K10" s="20">
-        <v>0</v>
-      </c>
-      <c r="L10" s="20"/>
+      <c r="K10" s="19">
+        <v>0</v>
+      </c>
+      <c r="L10" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="19" t="s">
+      <c r="B11" s="61"/>
+      <c r="C11" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="17">
         <v>12</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <v>8</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="19">
         <v>4</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="19">
         <v>2</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="19">
         <v>1</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="19">
         <v>1</v>
       </c>
-      <c r="K11" s="20">
-        <v>0</v>
-      </c>
-      <c r="L11" s="20"/>
+      <c r="K11" s="19">
+        <v>0</v>
+      </c>
+      <c r="L11" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="19" t="s">
+      <c r="B12" s="47"/>
+      <c r="C12" s="18" t="s">
         <v>75</v>
       </c>
       <c r="D12" s="16" t="s">
@@ -3446,29 +3514,31 @@
       <c r="F12" s="15">
         <v>6</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="22">
         <v>3</v>
       </c>
-      <c r="H12" s="23">
+      <c r="H12" s="22">
         <v>1</v>
       </c>
-      <c r="I12" s="23">
+      <c r="I12" s="22">
         <v>1</v>
       </c>
-      <c r="J12" s="23">
+      <c r="J12" s="22">
         <v>1</v>
       </c>
-      <c r="K12" s="23">
-        <v>0</v>
-      </c>
-      <c r="L12" s="20"/>
+      <c r="K12" s="22">
+        <v>0</v>
+      </c>
+      <c r="L12" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="18" t="s">
         <v>76</v>
       </c>
       <c r="D13" s="16" t="s">
@@ -3480,156 +3550,164 @@
       <c r="F13" s="15">
         <v>4</v>
       </c>
-      <c r="G13" s="23">
+      <c r="G13" s="22">
         <v>3</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="22">
         <v>1</v>
       </c>
-      <c r="I13" s="23">
-        <v>0</v>
-      </c>
-      <c r="J13" s="23">
-        <v>0</v>
-      </c>
-      <c r="K13" s="23">
-        <v>0</v>
-      </c>
-      <c r="L13" s="20"/>
+      <c r="I13" s="22">
+        <v>0</v>
+      </c>
+      <c r="J13" s="22">
+        <v>0</v>
+      </c>
+      <c r="K13" s="22">
+        <v>0</v>
+      </c>
+      <c r="L13" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
-      <c r="B14" s="41"/>
-      <c r="C14" s="19" t="s">
+      <c r="B14" s="47"/>
+      <c r="C14" s="18" t="s">
         <v>77</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="17">
         <v>10</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="17">
         <v>9</v>
       </c>
-      <c r="G14" s="20">
+      <c r="G14" s="19">
         <v>5</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="19">
         <v>2</v>
       </c>
-      <c r="I14" s="20">
-        <v>0</v>
-      </c>
-      <c r="J14" s="20">
-        <v>0</v>
-      </c>
-      <c r="K14" s="23">
-        <v>0</v>
-      </c>
-      <c r="L14" s="20"/>
+      <c r="I14" s="19">
+        <v>0</v>
+      </c>
+      <c r="J14" s="19">
+        <v>0</v>
+      </c>
+      <c r="K14" s="22">
+        <v>0</v>
+      </c>
+      <c r="L14" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="21" t="s">
+      <c r="C15" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D15" s="42" t="s">
+      <c r="D15" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="46">
         <v>5</v>
       </c>
-      <c r="F15" s="40">
+      <c r="F15" s="46">
         <v>4</v>
       </c>
-      <c r="G15" s="58">
+      <c r="G15" s="65">
         <v>3</v>
       </c>
-      <c r="H15" s="58">
+      <c r="H15" s="65">
         <v>2</v>
       </c>
-      <c r="I15" s="58">
+      <c r="I15" s="65">
         <v>1</v>
       </c>
-      <c r="J15" s="58">
-        <v>0</v>
-      </c>
-      <c r="K15" s="50">
-        <v>0</v>
-      </c>
-      <c r="L15" s="56"/>
+      <c r="J15" s="65">
+        <v>0</v>
+      </c>
+      <c r="K15" s="56">
+        <v>0</v>
+      </c>
+      <c r="L15" s="63">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="22" t="s">
+      <c r="B16" s="61"/>
+      <c r="C16" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="57"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="64"/>
     </row>
     <row r="17" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
-      <c r="B17" s="54"/>
-      <c r="C17" s="21" t="s">
+      <c r="B17" s="61"/>
+      <c r="C17" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="42" t="s">
+      <c r="D17" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="E17" s="40">
+      <c r="E17" s="46">
         <v>15</v>
       </c>
-      <c r="F17" s="40">
+      <c r="F17" s="46">
         <v>15</v>
       </c>
-      <c r="G17" s="58">
+      <c r="G17" s="65">
         <v>12</v>
       </c>
-      <c r="H17" s="58">
+      <c r="H17" s="65">
         <v>10</v>
       </c>
-      <c r="I17" s="58">
+      <c r="I17" s="65">
         <v>8</v>
       </c>
-      <c r="J17" s="58">
+      <c r="J17" s="65">
         <v>7</v>
       </c>
-      <c r="K17" s="50">
+      <c r="K17" s="56">
         <v>5</v>
       </c>
-      <c r="L17" s="56"/>
+      <c r="L17" s="63">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="22" t="s">
+      <c r="B18" s="61"/>
+      <c r="C18" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="50"/>
-      <c r="L18" s="57"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="64"/>
     </row>
     <row r="19" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
-      <c r="B19" s="41"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="16" t="s">
         <v>82</v>
       </c>
@@ -3642,22 +3720,24 @@
       <c r="F19" s="15">
         <v>6</v>
       </c>
-      <c r="G19" s="23">
+      <c r="G19" s="22">
         <v>5</v>
       </c>
-      <c r="H19" s="23">
+      <c r="H19" s="22">
         <v>4</v>
       </c>
-      <c r="I19" s="23">
+      <c r="I19" s="22">
         <v>3</v>
       </c>
-      <c r="J19" s="23">
+      <c r="J19" s="22">
         <v>2</v>
       </c>
-      <c r="K19" s="23">
-        <v>0</v>
-      </c>
-      <c r="L19" s="20"/>
+      <c r="K19" s="22">
+        <v>0</v>
+      </c>
+      <c r="L19" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
@@ -3667,21 +3747,33 @@
       <c r="C20" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="17">
         <v>25</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="17">
         <v>23</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
+      <c r="G20" s="19">
+        <v>20</v>
+      </c>
+      <c r="H20" s="19">
+        <v>18</v>
+      </c>
+      <c r="I20" s="19">
+        <v>17</v>
+      </c>
+      <c r="J20" s="19">
+        <v>12</v>
+      </c>
+      <c r="K20" s="19">
+        <v>8</v>
+      </c>
+      <c r="L20" s="36">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
@@ -3691,31 +3783,33 @@
       <c r="C21" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="17">
         <v>5</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="17">
         <v>5</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="19">
         <v>5</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="19">
         <v>5</v>
       </c>
-      <c r="I21" s="20">
+      <c r="I21" s="19">
         <v>2</v>
       </c>
-      <c r="J21" s="20">
+      <c r="J21" s="19">
         <v>2</v>
       </c>
-      <c r="K21" s="20">
-        <v>0</v>
-      </c>
-      <c r="L21" s="20"/>
+      <c r="K21" s="19">
+        <v>0</v>
+      </c>
+      <c r="L21" s="36">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
@@ -3725,31 +3819,33 @@
       <c r="C22" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="17">
         <v>5</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="17">
         <v>5</v>
       </c>
-      <c r="G22" s="20">
+      <c r="G22" s="19">
         <v>5</v>
       </c>
-      <c r="H22" s="20">
+      <c r="H22" s="19">
         <v>5</v>
       </c>
-      <c r="I22" s="20">
-        <v>0</v>
-      </c>
-      <c r="J22" s="20">
-        <v>0</v>
-      </c>
-      <c r="K22" s="20">
-        <v>0</v>
-      </c>
-      <c r="L22" s="20"/>
+      <c r="I22" s="19">
+        <v>0</v>
+      </c>
+      <c r="J22" s="19">
+        <v>0</v>
+      </c>
+      <c r="K22" s="19">
+        <v>0</v>
+      </c>
+      <c r="L22" s="36">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
start of sprint #3 - backlog updated
</commit_message>
<xml_diff>
--- a/process/Project Backlog.xlsx
+++ b/process/Project Backlog.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardoperugini/Desktop/PPS-19-Primer/process/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49CB7E2-7468-7849-B1C0-C2CA3E1C9E71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1646D0-57E1-A241-BAE6-CB5CB5632391}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13020" yWindow="460" windowWidth="15780" windowHeight="16760" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13020" yWindow="460" windowWidth="15780" windowHeight="16760" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Riepilogo di esportazione" sheetId="1" r:id="rId1"/>
     <sheet name="Product Backlog" sheetId="2" r:id="rId2"/>
     <sheet name="1 Sprint Backlog" sheetId="3" r:id="rId3"/>
     <sheet name="2 Sprint Backlog" sheetId="4" r:id="rId4"/>
+    <sheet name="3 Sprint Backlog" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="108">
   <si>
     <t>Questo documento è stato esportato da Numbers. Tutte le tabelle sono state convertite in un foglio di lavoro di Excel. Tutti gli altri oggetti di ciascun foglio di Numbers sono stati collocati in fogli di lavoro separati. Nota che i calcoli delle formule potrebbero differire in Excel.</t>
   </si>
@@ -112,9 +113,6 @@
     <t>e conseguente implementazione</t>
   </si>
   <si>
-    <t xml:space="preserve">Refactoring </t>
-  </si>
-  <si>
     <t>Rimozione codice duplicato e rimozione debito tecnico</t>
   </si>
   <si>
@@ -284,6 +282,72 @@
   </si>
   <si>
     <t>Refctoring della factory per sviluppo collezione di creature e food</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Aggiunta di strumenti per pulizia del codice</t>
+  </si>
+  <si>
+    <t>Tuning dei parametri di simulazione</t>
+  </si>
+  <si>
+    <t>GUI display improvement</t>
+  </si>
+  <si>
+    <t>ScalaDoc refactoring</t>
+  </si>
+  <si>
+    <t>Full functional test refactoring</t>
+  </si>
+  <si>
+    <t>Full functional GUI refactoring</t>
+  </si>
+  <si>
+    <t>Full functional controller refactoring</t>
+  </si>
+  <si>
+    <t>Refactoring</t>
+  </si>
+  <si>
+    <t>Aggiunta 'tolleranza' collisioni (sense)</t>
+  </si>
+  <si>
+    <t>Calcolo della nuova posizione verso il goal</t>
+  </si>
+  <si>
+    <t>Sviluppo movimento</t>
+  </si>
+  <si>
+    <t>Integrazione di una nuova libreria cats-effect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrazione </t>
+  </si>
+  <si>
+    <t>Sviluppo Movimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Functional Refactoring </t>
+  </si>
+  <si>
+    <t>Sostituzione della libreria scalaz-io-effect con la libreria cats-effect</t>
+  </si>
+  <si>
+    <t>Integrazione nuova libreria</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Sviluppo di un meccanismo per il movimento rettilineo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> dei blob all'interno dell'environment verso il proprio goal</t>
+  </si>
+  <si>
+    <t>F/L</t>
   </si>
 </sst>
 </file>
@@ -349,7 +413,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -597,11 +661,148 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -628,12 +829,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -707,22 +902,19 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -740,19 +932,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -776,9 +971,106 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{D72B9B27-414B-F844-8B5D-35F2FE6FE4EE}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1947,11 +2239,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
+      <c r="B3" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="7" spans="2:4" ht="19" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -1982,7 +2274,7 @@
     </row>
     <row r="11" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -1993,12 +2285,12 @@
         <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -2009,7 +2301,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2027,10 +2319,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+    <sheetView showGridLines="0" zoomScale="83" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2045,12 +2337,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2088,472 +2380,542 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="50"/>
-      <c r="H4" s="50"/>
-      <c r="I4" s="50"/>
-      <c r="J4" s="51"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="48"/>
     </row>
     <row r="5" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="87" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="88">
         <v>1</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="88">
         <v>2</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="88">
         <v>3</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="88">
         <v>4</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="88">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15">
+    <row r="6" spans="1:10" s="86" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="85"/>
+      <c r="B6" s="95">
         <v>1</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="37">
-        <v>20</v>
-      </c>
-      <c r="F6" s="37">
-        <v>20</v>
-      </c>
-      <c r="G6" s="38">
+      <c r="C6" s="94" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="94" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="94" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="95">
+        <v>10</v>
+      </c>
+      <c r="G6" s="95">
+        <v>10</v>
+      </c>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+    </row>
+    <row r="7" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="B7" s="89">
+        <v>2</v>
+      </c>
+      <c r="C7" s="90" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="91" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="92">
         <v>5</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17">
-        <v>2</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="39">
-        <v>7</v>
-      </c>
-      <c r="F7" s="39">
-        <v>7</v>
-      </c>
-      <c r="G7" s="40">
-        <v>1</v>
-      </c>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
-      <c r="J7" s="40"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="46">
+      <c r="F7" s="92">
+        <v>5</v>
+      </c>
+      <c r="G7" s="93">
+        <v>5</v>
+      </c>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+    </row>
+    <row r="8" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="97" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="12"/>
+      <c r="B9" s="15">
         <v>3</v>
       </c>
-      <c r="C8" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="20" t="s">
+      <c r="C9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="37">
         <v>17</v>
       </c>
-      <c r="E8" s="45">
-        <v>8</v>
-      </c>
-      <c r="F8" s="45">
-        <v>8</v>
-      </c>
-      <c r="G8" s="43">
-        <v>1</v>
-      </c>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="47"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
+      <c r="F9" s="37">
+        <v>17</v>
+      </c>
+      <c r="G9" s="38">
+        <v>17</v>
+      </c>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
     </row>
     <row r="10" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="15">
         <v>4</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>19</v>
+      <c r="C10" s="96" t="s">
+        <v>101</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="E10" s="37">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F10" s="37">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" s="38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
       <c r="J10" s="38"/>
     </row>
     <row r="11" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="46">
+      <c r="A11" s="12"/>
+      <c r="B11" s="15">
         <v>5</v>
       </c>
-      <c r="C11" s="48" t="s">
+      <c r="C11" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" s="37">
+        <v>5</v>
+      </c>
+      <c r="F11" s="37">
+        <v>5</v>
+      </c>
+      <c r="G11" s="38">
+        <v>5</v>
+      </c>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="15">
+        <v>6</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="37">
+        <v>5</v>
+      </c>
+      <c r="F12" s="37">
+        <v>5</v>
+      </c>
+      <c r="G12" s="38">
+        <v>5</v>
+      </c>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="15">
+        <v>7</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="35">
+        <v>30</v>
+      </c>
+      <c r="F13" s="35">
+        <v>25</v>
+      </c>
+      <c r="G13" s="36">
+        <v>20</v>
+      </c>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+    </row>
+    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="15">
+        <v>8</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="35">
+        <v>20</v>
+      </c>
+      <c r="F14" s="35">
+        <v>20</v>
+      </c>
+      <c r="G14" s="36">
+        <v>2</v>
+      </c>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="15">
+        <v>9</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="35">
+        <v>11</v>
+      </c>
+      <c r="F15" s="35">
+        <v>11</v>
+      </c>
+      <c r="G15" s="36">
+        <v>2</v>
+      </c>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="15">
+        <v>10</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="37">
+        <v>7</v>
+      </c>
+      <c r="F16" s="37">
+        <v>7</v>
+      </c>
+      <c r="G16" s="38">
+        <v>1</v>
+      </c>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="51">
+        <v>11</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="54">
+        <v>8</v>
+      </c>
+      <c r="F17" s="54">
+        <v>8</v>
+      </c>
+      <c r="G17" s="56">
+        <v>1</v>
+      </c>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="55"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="51">
+        <v>12</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="54">
+        <v>7</v>
+      </c>
+      <c r="F19" s="54">
+        <v>2</v>
+      </c>
+      <c r="G19" s="56">
+        <v>1</v>
+      </c>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
+    </row>
+    <row r="20" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="55"/>
+      <c r="F20" s="55"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
+    </row>
+    <row r="21" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="89">
+        <v>13</v>
+      </c>
+      <c r="C21" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D21" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="45">
+      <c r="E21" s="92">
         <v>15</v>
       </c>
-      <c r="F11" s="45">
+      <c r="F21" s="92">
         <v>15</v>
       </c>
-      <c r="G11" s="43">
-        <v>0</v>
-      </c>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="21" t="s">
+      <c r="G21" s="93">
+        <v>0</v>
+      </c>
+      <c r="H21" s="93"/>
+      <c r="I21" s="93"/>
+      <c r="J21" s="93"/>
+    </row>
+    <row r="22" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="52"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="15">
-        <v>6</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="37">
-        <v>30</v>
-      </c>
-      <c r="F13" s="37">
-        <v>25</v>
-      </c>
-      <c r="G13" s="38">
-        <v>20</v>
-      </c>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="46">
-        <v>7</v>
-      </c>
-      <c r="C14" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="45">
-        <v>7</v>
-      </c>
-      <c r="F14" s="45">
-        <v>2</v>
-      </c>
-      <c r="G14" s="43">
-        <v>1</v>
-      </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="47"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="17">
-        <v>8</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="39">
-        <v>10</v>
-      </c>
-      <c r="F16" s="39">
-        <v>10</v>
-      </c>
-      <c r="G16" s="40">
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="55"/>
+    </row>
+    <row r="23" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+      <c r="B23" s="42">
+        <v>14</v>
+      </c>
+      <c r="C23" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="45">
+        <v>5</v>
+      </c>
+      <c r="F23" s="45">
+        <v>0</v>
+      </c>
+      <c r="G23" s="41">
+        <v>0</v>
+      </c>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+    </row>
+    <row r="24" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="12"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="41"/>
+      <c r="J24" s="41"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="12"/>
+      <c r="B25" s="13">
+        <v>15</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E25" s="35">
         <v>3</v>
       </c>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="17">
-        <v>9</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="39">
-        <v>17</v>
-      </c>
-      <c r="F17" s="39">
-        <v>17</v>
-      </c>
-      <c r="G17" s="40">
-        <v>17</v>
-      </c>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="17">
-        <v>10</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="39">
-        <v>5</v>
-      </c>
-      <c r="F18" s="39">
-        <v>5</v>
-      </c>
-      <c r="G18" s="40">
-        <v>5</v>
-      </c>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="17">
-        <v>11</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="39">
-        <v>5</v>
-      </c>
-      <c r="F19" s="39">
-        <v>5</v>
-      </c>
-      <c r="G19" s="40">
-        <v>5</v>
-      </c>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-    </row>
-    <row r="20" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="55">
-        <v>12</v>
-      </c>
-      <c r="C20" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="58">
-        <v>5</v>
-      </c>
-      <c r="F20" s="58">
-        <v>0</v>
-      </c>
-      <c r="G20" s="54">
-        <v>0</v>
-      </c>
-      <c r="H20" s="54"/>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
-    </row>
-    <row r="21" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="54"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="54"/>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-    </row>
-    <row r="22" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="15">
-        <v>13</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="16" t="s">
+      <c r="F25" s="35">
+        <v>0</v>
+      </c>
+      <c r="G25" s="36">
+        <v>0</v>
+      </c>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+    </row>
+    <row r="26" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="12"/>
+      <c r="B26" s="13">
+        <v>16</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="37">
-        <v>3</v>
-      </c>
-      <c r="F22" s="37">
-        <v>0</v>
-      </c>
-      <c r="G22" s="38">
-        <v>0</v>
-      </c>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-    </row>
-    <row r="23" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="15">
-        <v>14</v>
-      </c>
-      <c r="C23" s="16" t="s">
+      <c r="D26" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="37">
+      <c r="E26" s="35">
         <v>4</v>
       </c>
-      <c r="F23" s="37">
-        <v>0</v>
-      </c>
-      <c r="G23" s="38">
-        <v>0</v>
-      </c>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
+      <c r="F26" s="35">
+        <v>0</v>
+      </c>
+      <c r="G26" s="36">
+        <v>0</v>
+      </c>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
+  <mergeCells count="42">
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="E17:E18"/>
     <mergeCell ref="F4:J4"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -2573,22 +2935,22 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="23" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" style="23" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" style="23" customWidth="1"/>
-    <col min="6" max="12" width="10.83203125" style="23" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="23"/>
+    <col min="1" max="1" width="10.83203125" style="21" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="21" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" style="21" customWidth="1"/>
+    <col min="6" max="12" width="10.83203125" style="21" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2641,583 +3003,583 @@
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="60"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="58"/>
     </row>
     <row r="6" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="D6" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="E6" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="F6" s="24">
+        <v>1</v>
+      </c>
+      <c r="G6" s="24">
+        <v>2</v>
+      </c>
+      <c r="H6" s="24">
+        <v>3</v>
+      </c>
+      <c r="I6" s="24">
+        <v>4</v>
+      </c>
+      <c r="J6" s="24">
+        <v>5</v>
+      </c>
+      <c r="K6" s="24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12"/>
+      <c r="B7" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="26">
+      <c r="D7" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="27">
+        <v>7</v>
+      </c>
+      <c r="F7" s="27">
         <v>1</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G7" s="27">
+        <v>1</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0</v>
+      </c>
+      <c r="I7" s="27">
+        <v>0</v>
+      </c>
+      <c r="J7" s="27">
+        <v>0</v>
+      </c>
+      <c r="K7" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="13">
+        <v>3</v>
+      </c>
+      <c r="F8" s="13">
+        <v>1</v>
+      </c>
+      <c r="G8" s="13">
+        <v>1</v>
+      </c>
+      <c r="H8" s="13">
+        <v>0</v>
+      </c>
+      <c r="I8" s="13">
+        <v>0</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0</v>
+      </c>
+      <c r="K8" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="12"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="13">
+        <v>3</v>
+      </c>
+      <c r="F9" s="13">
+        <v>1</v>
+      </c>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
+      <c r="H9" s="13">
+        <v>0</v>
+      </c>
+      <c r="I9" s="13">
+        <v>0</v>
+      </c>
+      <c r="J9" s="13">
+        <v>0</v>
+      </c>
+      <c r="K9" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="13">
+        <v>7</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+      <c r="H10" s="13">
+        <v>0</v>
+      </c>
+      <c r="I10" s="13">
+        <v>0</v>
+      </c>
+      <c r="J10" s="13">
+        <v>0</v>
+      </c>
+      <c r="K10" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="13">
+        <v>7</v>
+      </c>
+      <c r="F11" s="13">
+        <v>1</v>
+      </c>
+      <c r="G11" s="13">
+        <v>1</v>
+      </c>
+      <c r="H11" s="13">
+        <v>0</v>
+      </c>
+      <c r="I11" s="13">
+        <v>0</v>
+      </c>
+      <c r="J11" s="13">
+        <v>0</v>
+      </c>
+      <c r="K11" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="13">
+        <v>15</v>
+      </c>
+      <c r="F12" s="13">
+        <v>12</v>
+      </c>
+      <c r="G12" s="13">
+        <v>10</v>
+      </c>
+      <c r="H12" s="13">
+        <v>10</v>
+      </c>
+      <c r="I12" s="13">
+        <v>10</v>
+      </c>
+      <c r="J12" s="13">
+        <v>10</v>
+      </c>
+      <c r="K12" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="13">
         <v>2</v>
       </c>
-      <c r="H6" s="26">
+      <c r="F13" s="13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="13">
+        <v>0</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="13">
         <v>3</v>
       </c>
-      <c r="I6" s="26">
+      <c r="F14" s="13">
+        <v>0</v>
+      </c>
+      <c r="G14" s="13">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13">
+        <v>0</v>
+      </c>
+      <c r="I14" s="13">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0</v>
+      </c>
+      <c r="K14" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="13">
+        <v>2</v>
+      </c>
+      <c r="F15" s="13">
+        <v>0</v>
+      </c>
+      <c r="G15" s="13">
+        <v>0</v>
+      </c>
+      <c r="H15" s="13">
+        <v>0</v>
+      </c>
+      <c r="I15" s="13">
+        <v>0</v>
+      </c>
+      <c r="J15" s="13">
+        <v>0</v>
+      </c>
+      <c r="K15" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="13">
+        <v>2</v>
+      </c>
+      <c r="F16" s="13">
+        <v>0</v>
+      </c>
+      <c r="G16" s="13">
+        <v>0</v>
+      </c>
+      <c r="H16" s="13">
+        <v>0</v>
+      </c>
+      <c r="I16" s="13">
+        <v>0</v>
+      </c>
+      <c r="J16" s="13">
+        <v>0</v>
+      </c>
+      <c r="K16" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="13">
+        <v>2</v>
+      </c>
+      <c r="F17" s="13">
+        <v>0</v>
+      </c>
+      <c r="G17" s="13">
+        <v>0</v>
+      </c>
+      <c r="H17" s="13">
+        <v>0</v>
+      </c>
+      <c r="I17" s="13">
+        <v>0</v>
+      </c>
+      <c r="J17" s="13">
+        <v>0</v>
+      </c>
+      <c r="K17" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="13">
+        <v>3</v>
+      </c>
+      <c r="F18" s="13">
+        <v>3</v>
+      </c>
+      <c r="G18" s="13">
+        <v>3</v>
+      </c>
+      <c r="H18" s="13">
+        <v>2</v>
+      </c>
+      <c r="I18" s="13">
+        <v>0</v>
+      </c>
+      <c r="J18" s="13">
+        <v>0</v>
+      </c>
+      <c r="K18" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="13">
+        <v>3</v>
+      </c>
+      <c r="F19" s="13">
+        <v>3</v>
+      </c>
+      <c r="G19" s="13">
+        <v>3</v>
+      </c>
+      <c r="H19" s="13">
+        <v>2</v>
+      </c>
+      <c r="I19" s="13">
+        <v>0</v>
+      </c>
+      <c r="J19" s="13">
+        <v>0</v>
+      </c>
+      <c r="K19" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="13">
         <v>4</v>
       </c>
-      <c r="J6" s="26">
+      <c r="F20" s="13">
+        <v>2</v>
+      </c>
+      <c r="G20" s="13">
+        <v>2</v>
+      </c>
+      <c r="H20" s="13">
+        <v>0</v>
+      </c>
+      <c r="I20" s="13">
+        <v>0</v>
+      </c>
+      <c r="J20" s="13">
+        <v>0</v>
+      </c>
+      <c r="K20" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="59"/>
+      <c r="C21" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="13">
         <v>5</v>
       </c>
-      <c r="K6" s="26">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="62" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="27" t="s">
+      <c r="F21" s="13">
+        <v>3</v>
+      </c>
+      <c r="G21" s="13">
+        <v>1</v>
+      </c>
+      <c r="H21" s="13">
+        <v>0</v>
+      </c>
+      <c r="I21" s="13">
+        <v>0</v>
+      </c>
+      <c r="J21" s="13">
+        <v>0</v>
+      </c>
+      <c r="K21" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="59"/>
+      <c r="C22" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" s="13">
+        <v>5</v>
+      </c>
+      <c r="F22" s="13">
+        <v>3</v>
+      </c>
+      <c r="G22" s="13">
+        <v>1</v>
+      </c>
+      <c r="H22" s="13">
+        <v>0</v>
+      </c>
+      <c r="I22" s="13">
+        <v>0</v>
+      </c>
+      <c r="J22" s="13">
+        <v>0</v>
+      </c>
+      <c r="K22" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="29">
-        <v>7</v>
-      </c>
-      <c r="F7" s="29">
+      <c r="E23" s="13">
+        <v>5</v>
+      </c>
+      <c r="F23" s="13">
+        <v>4</v>
+      </c>
+      <c r="G23" s="13">
+        <v>3</v>
+      </c>
+      <c r="H23" s="13">
+        <v>3</v>
+      </c>
+      <c r="I23" s="13">
+        <v>2</v>
+      </c>
+      <c r="J23" s="13">
         <v>1</v>
       </c>
-      <c r="G7" s="29">
-        <v>1</v>
-      </c>
-      <c r="H7" s="29">
-        <v>0</v>
-      </c>
-      <c r="I7" s="29">
-        <v>0</v>
-      </c>
-      <c r="J7" s="29">
-        <v>0</v>
-      </c>
-      <c r="K7" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="15">
-        <v>3</v>
-      </c>
-      <c r="F8" s="15">
-        <v>1</v>
-      </c>
-      <c r="G8" s="15">
-        <v>1</v>
-      </c>
-      <c r="H8" s="15">
-        <v>0</v>
-      </c>
-      <c r="I8" s="15">
-        <v>0</v>
-      </c>
-      <c r="J8" s="15">
-        <v>0</v>
-      </c>
-      <c r="K8" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="15">
-        <v>3</v>
-      </c>
-      <c r="F9" s="15">
-        <v>1</v>
-      </c>
-      <c r="G9" s="15">
-        <v>1</v>
-      </c>
-      <c r="H9" s="15">
-        <v>0</v>
-      </c>
-      <c r="I9" s="15">
-        <v>0</v>
-      </c>
-      <c r="J9" s="15">
-        <v>0</v>
-      </c>
-      <c r="K9" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="15">
-        <v>7</v>
-      </c>
-      <c r="F10" s="15">
-        <v>1</v>
-      </c>
-      <c r="G10" s="15">
-        <v>1</v>
-      </c>
-      <c r="H10" s="15">
-        <v>0</v>
-      </c>
-      <c r="I10" s="15">
-        <v>0</v>
-      </c>
-      <c r="J10" s="15">
-        <v>0</v>
-      </c>
-      <c r="K10" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="47"/>
-      <c r="C11" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="15">
-        <v>7</v>
-      </c>
-      <c r="F11" s="15">
-        <v>1</v>
-      </c>
-      <c r="G11" s="15">
-        <v>1</v>
-      </c>
-      <c r="H11" s="15">
-        <v>0</v>
-      </c>
-      <c r="I11" s="15">
-        <v>0</v>
-      </c>
-      <c r="J11" s="15">
-        <v>0</v>
-      </c>
-      <c r="K11" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="15">
-        <v>15</v>
-      </c>
-      <c r="F12" s="15">
-        <v>12</v>
-      </c>
-      <c r="G12" s="15">
-        <v>10</v>
-      </c>
-      <c r="H12" s="15">
-        <v>10</v>
-      </c>
-      <c r="I12" s="15">
-        <v>10</v>
-      </c>
-      <c r="J12" s="15">
-        <v>10</v>
-      </c>
-      <c r="K12" s="15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="15">
-        <v>2</v>
-      </c>
-      <c r="F13" s="15">
-        <v>0</v>
-      </c>
-      <c r="G13" s="15">
-        <v>0</v>
-      </c>
-      <c r="H13" s="15">
-        <v>0</v>
-      </c>
-      <c r="I13" s="15">
-        <v>0</v>
-      </c>
-      <c r="J13" s="15">
-        <v>0</v>
-      </c>
-      <c r="K13" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="15">
-        <v>3</v>
-      </c>
-      <c r="F14" s="15">
-        <v>0</v>
-      </c>
-      <c r="G14" s="15">
-        <v>0</v>
-      </c>
-      <c r="H14" s="15">
-        <v>0</v>
-      </c>
-      <c r="I14" s="15">
-        <v>0</v>
-      </c>
-      <c r="J14" s="15">
-        <v>0</v>
-      </c>
-      <c r="K14" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="15">
-        <v>2</v>
-      </c>
-      <c r="F15" s="15">
-        <v>0</v>
-      </c>
-      <c r="G15" s="15">
-        <v>0</v>
-      </c>
-      <c r="H15" s="15">
-        <v>0</v>
-      </c>
-      <c r="I15" s="15">
-        <v>0</v>
-      </c>
-      <c r="J15" s="15">
-        <v>0</v>
-      </c>
-      <c r="K15" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="61"/>
-      <c r="C16" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="15">
-        <v>2</v>
-      </c>
-      <c r="F16" s="15">
-        <v>0</v>
-      </c>
-      <c r="G16" s="15">
-        <v>0</v>
-      </c>
-      <c r="H16" s="15">
-        <v>0</v>
-      </c>
-      <c r="I16" s="15">
-        <v>0</v>
-      </c>
-      <c r="J16" s="15">
-        <v>0</v>
-      </c>
-      <c r="K16" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="15">
-        <v>2</v>
-      </c>
-      <c r="F17" s="15">
-        <v>0</v>
-      </c>
-      <c r="G17" s="15">
-        <v>0</v>
-      </c>
-      <c r="H17" s="15">
-        <v>0</v>
-      </c>
-      <c r="I17" s="15">
-        <v>0</v>
-      </c>
-      <c r="J17" s="15">
-        <v>0</v>
-      </c>
-      <c r="K17" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="15">
-        <v>3</v>
-      </c>
-      <c r="F18" s="15">
-        <v>3</v>
-      </c>
-      <c r="G18" s="15">
-        <v>3</v>
-      </c>
-      <c r="H18" s="15">
-        <v>2</v>
-      </c>
-      <c r="I18" s="15">
-        <v>0</v>
-      </c>
-      <c r="J18" s="15">
-        <v>0</v>
-      </c>
-      <c r="K18" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="15">
-        <v>3</v>
-      </c>
-      <c r="F19" s="15">
-        <v>3</v>
-      </c>
-      <c r="G19" s="15">
-        <v>3</v>
-      </c>
-      <c r="H19" s="15">
-        <v>2</v>
-      </c>
-      <c r="I19" s="15">
-        <v>0</v>
-      </c>
-      <c r="J19" s="15">
-        <v>0</v>
-      </c>
-      <c r="K19" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="15">
-        <v>4</v>
-      </c>
-      <c r="F20" s="15">
-        <v>2</v>
-      </c>
-      <c r="G20" s="15">
-        <v>2</v>
-      </c>
-      <c r="H20" s="15">
-        <v>0</v>
-      </c>
-      <c r="I20" s="15">
-        <v>0</v>
-      </c>
-      <c r="J20" s="15">
-        <v>0</v>
-      </c>
-      <c r="K20" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="15">
-        <v>5</v>
-      </c>
-      <c r="F21" s="15">
-        <v>3</v>
-      </c>
-      <c r="G21" s="15">
-        <v>1</v>
-      </c>
-      <c r="H21" s="15">
-        <v>0</v>
-      </c>
-      <c r="I21" s="15">
-        <v>0</v>
-      </c>
-      <c r="J21" s="15">
-        <v>0</v>
-      </c>
-      <c r="K21" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="30" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="15">
-        <v>5</v>
-      </c>
-      <c r="F22" s="15">
-        <v>3</v>
-      </c>
-      <c r="G22" s="15">
-        <v>1</v>
-      </c>
-      <c r="H22" s="15">
-        <v>0</v>
-      </c>
-      <c r="I22" s="15">
-        <v>0</v>
-      </c>
-      <c r="J22" s="15">
-        <v>0</v>
-      </c>
-      <c r="K22" s="15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="47"/>
-      <c r="C23" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="15">
-        <v>5</v>
-      </c>
-      <c r="F23" s="15">
-        <v>4</v>
-      </c>
-      <c r="G23" s="15">
-        <v>3</v>
-      </c>
-      <c r="H23" s="15">
-        <v>3</v>
-      </c>
-      <c r="I23" s="15">
-        <v>2</v>
-      </c>
-      <c r="J23" s="15">
-        <v>1</v>
-      </c>
-      <c r="K23" s="15">
+      <c r="K23" s="13">
         <v>1</v>
       </c>
     </row>
@@ -3242,28 +3604,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="31" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="31" customWidth="1"/>
-    <col min="3" max="3" width="63.1640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" style="31" customWidth="1"/>
-    <col min="5" max="5" width="21.1640625" style="31" customWidth="1"/>
-    <col min="6" max="13" width="10.83203125" style="31" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="31"/>
+    <col min="1" max="1" width="10.83203125" style="29" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="29" customWidth="1"/>
+    <col min="3" max="3" width="63.1640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" style="29" customWidth="1"/>
+    <col min="5" max="5" width="21.1640625" style="29" customWidth="1"/>
+    <col min="6" max="13" width="10.83203125" style="29" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -3348,507 +3710,515 @@
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="49" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="60"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="57"/>
+      <c r="H7" s="57"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="57"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="58"/>
     </row>
     <row r="8" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="D8" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="E8" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8" s="26">
+      <c r="F8" s="24">
         <v>1</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="24">
         <v>2</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="24">
         <v>3</v>
       </c>
-      <c r="I8" s="26">
+      <c r="I8" s="24">
         <v>4</v>
       </c>
-      <c r="J8" s="26">
+      <c r="J8" s="24">
         <v>5</v>
       </c>
-      <c r="K8" s="26">
+      <c r="K8" s="24">
         <v>6</v>
       </c>
-      <c r="L8" s="26">
+      <c r="L8" s="24">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="62" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="28" t="s">
+      <c r="E9" s="31">
+        <v>5</v>
+      </c>
+      <c r="F9" s="31">
+        <v>3</v>
+      </c>
+      <c r="G9" s="32">
+        <v>2</v>
+      </c>
+      <c r="H9" s="32">
+        <v>1</v>
+      </c>
+      <c r="I9" s="32">
+        <v>1</v>
+      </c>
+      <c r="J9" s="32">
+        <v>1</v>
+      </c>
+      <c r="K9" s="32">
+        <v>0</v>
+      </c>
+      <c r="L9" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E9" s="33">
+      <c r="D10" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="15">
+        <v>10</v>
+      </c>
+      <c r="F10" s="15">
+        <v>6</v>
+      </c>
+      <c r="G10" s="17">
+        <v>3</v>
+      </c>
+      <c r="H10" s="17">
+        <v>1</v>
+      </c>
+      <c r="I10" s="17">
+        <v>1</v>
+      </c>
+      <c r="J10" s="17">
+        <v>1</v>
+      </c>
+      <c r="K10" s="17">
+        <v>0</v>
+      </c>
+      <c r="L10" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="12"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="15">
+        <v>12</v>
+      </c>
+      <c r="F11" s="15">
+        <v>8</v>
+      </c>
+      <c r="G11" s="17">
+        <v>4</v>
+      </c>
+      <c r="H11" s="17">
+        <v>2</v>
+      </c>
+      <c r="I11" s="17">
+        <v>1</v>
+      </c>
+      <c r="J11" s="17">
+        <v>1</v>
+      </c>
+      <c r="K11" s="17">
+        <v>0</v>
+      </c>
+      <c r="L11" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="13">
+        <v>8</v>
+      </c>
+      <c r="F12" s="13">
+        <v>6</v>
+      </c>
+      <c r="G12" s="20">
+        <v>3</v>
+      </c>
+      <c r="H12" s="20">
+        <v>1</v>
+      </c>
+      <c r="I12" s="20">
+        <v>1</v>
+      </c>
+      <c r="J12" s="20">
+        <v>1</v>
+      </c>
+      <c r="K12" s="20">
+        <v>0</v>
+      </c>
+      <c r="L12" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="12"/>
+      <c r="B13" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="13">
         <v>5</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F13" s="13">
+        <v>4</v>
+      </c>
+      <c r="G13" s="20">
         <v>3</v>
       </c>
-      <c r="G9" s="34">
+      <c r="H13" s="20">
+        <v>1</v>
+      </c>
+      <c r="I13" s="20">
+        <v>0</v>
+      </c>
+      <c r="J13" s="20">
+        <v>0</v>
+      </c>
+      <c r="K13" s="20">
+        <v>0</v>
+      </c>
+      <c r="L13" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="12"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="15">
+        <v>10</v>
+      </c>
+      <c r="F14" s="15">
+        <v>9</v>
+      </c>
+      <c r="G14" s="17">
+        <v>5</v>
+      </c>
+      <c r="H14" s="17">
         <v>2</v>
       </c>
-      <c r="H9" s="34">
+      <c r="I14" s="17">
+        <v>0</v>
+      </c>
+      <c r="J14" s="17">
+        <v>0</v>
+      </c>
+      <c r="K14" s="20">
+        <v>0</v>
+      </c>
+      <c r="L14" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="B15" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="51">
+        <v>5</v>
+      </c>
+      <c r="F15" s="51">
+        <v>4</v>
+      </c>
+      <c r="G15" s="63">
+        <v>3</v>
+      </c>
+      <c r="H15" s="63">
+        <v>2</v>
+      </c>
+      <c r="I15" s="63">
         <v>1</v>
       </c>
-      <c r="I9" s="34">
-        <v>1</v>
-      </c>
-      <c r="J9" s="34">
-        <v>1</v>
-      </c>
-      <c r="K9" s="34">
-        <v>0</v>
-      </c>
-      <c r="L9" s="35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="17">
+      <c r="J15" s="63">
+        <v>0</v>
+      </c>
+      <c r="K15" s="43">
+        <v>0</v>
+      </c>
+      <c r="L15" s="61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="12"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="62"/>
+    </row>
+    <row r="17" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="12"/>
+      <c r="B17" s="59"/>
+      <c r="C17" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="53" t="s">
+        <v>67</v>
+      </c>
+      <c r="E17" s="51">
+        <v>15</v>
+      </c>
+      <c r="F17" s="51">
+        <v>15</v>
+      </c>
+      <c r="G17" s="63">
+        <v>12</v>
+      </c>
+      <c r="H17" s="63">
         <v>10</v>
       </c>
-      <c r="F10" s="17">
+      <c r="I17" s="63">
+        <v>8</v>
+      </c>
+      <c r="J17" s="63">
+        <v>7</v>
+      </c>
+      <c r="K17" s="43">
+        <v>5</v>
+      </c>
+      <c r="L17" s="61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="59"/>
+      <c r="C18" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="62"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="12"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="13">
+        <v>7</v>
+      </c>
+      <c r="F19" s="13">
         <v>6</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G19" s="20">
+        <v>5</v>
+      </c>
+      <c r="H19" s="20">
+        <v>4</v>
+      </c>
+      <c r="I19" s="20">
         <v>3</v>
       </c>
-      <c r="H10" s="19">
-        <v>1</v>
-      </c>
-      <c r="I10" s="19">
-        <v>1</v>
-      </c>
-      <c r="J10" s="19">
-        <v>1</v>
-      </c>
-      <c r="K10" s="19">
-        <v>0</v>
-      </c>
-      <c r="L10" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="17">
+      <c r="J19" s="20">
+        <v>2</v>
+      </c>
+      <c r="K19" s="20">
+        <v>0</v>
+      </c>
+      <c r="L19" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="B20" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="15">
+        <v>25</v>
+      </c>
+      <c r="F20" s="15">
+        <v>23</v>
+      </c>
+      <c r="G20" s="17">
+        <v>20</v>
+      </c>
+      <c r="H20" s="17">
+        <v>18</v>
+      </c>
+      <c r="I20" s="17">
+        <v>17</v>
+      </c>
+      <c r="J20" s="17">
         <v>12</v>
       </c>
-      <c r="F11" s="17">
+      <c r="K20" s="17">
         <v>8</v>
       </c>
-      <c r="G11" s="19">
-        <v>4</v>
-      </c>
-      <c r="H11" s="19">
+      <c r="L20" s="34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+      <c r="B21" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="15">
+        <v>5</v>
+      </c>
+      <c r="F21" s="15">
+        <v>5</v>
+      </c>
+      <c r="G21" s="17">
+        <v>5</v>
+      </c>
+      <c r="H21" s="17">
+        <v>5</v>
+      </c>
+      <c r="I21" s="17">
         <v>2</v>
       </c>
-      <c r="I11" s="19">
-        <v>1</v>
-      </c>
-      <c r="J11" s="19">
-        <v>1</v>
-      </c>
-      <c r="K11" s="19">
-        <v>0</v>
-      </c>
-      <c r="L11" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="15">
-        <v>8</v>
-      </c>
-      <c r="F12" s="15">
-        <v>6</v>
-      </c>
-      <c r="G12" s="22">
-        <v>3</v>
-      </c>
-      <c r="H12" s="22">
-        <v>1</v>
-      </c>
-      <c r="I12" s="22">
-        <v>1</v>
-      </c>
-      <c r="J12" s="22">
-        <v>1</v>
-      </c>
-      <c r="K12" s="22">
-        <v>0</v>
-      </c>
-      <c r="L12" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="15">
+      <c r="J21" s="17">
+        <v>2</v>
+      </c>
+      <c r="K21" s="17">
+        <v>0</v>
+      </c>
+      <c r="L21" s="34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="B22" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="15">
         <v>5</v>
       </c>
-      <c r="F13" s="15">
-        <v>4</v>
-      </c>
-      <c r="G13" s="22">
-        <v>3</v>
-      </c>
-      <c r="H13" s="22">
-        <v>1</v>
-      </c>
-      <c r="I13" s="22">
-        <v>0</v>
-      </c>
-      <c r="J13" s="22">
-        <v>0</v>
-      </c>
-      <c r="K13" s="22">
-        <v>0</v>
-      </c>
-      <c r="L13" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="17">
-        <v>10</v>
-      </c>
-      <c r="F14" s="17">
-        <v>9</v>
-      </c>
-      <c r="G14" s="19">
+      <c r="F22" s="15">
         <v>5</v>
       </c>
-      <c r="H14" s="19">
-        <v>2</v>
-      </c>
-      <c r="I14" s="19">
-        <v>0</v>
-      </c>
-      <c r="J14" s="19">
-        <v>0</v>
-      </c>
-      <c r="K14" s="22">
-        <v>0</v>
-      </c>
-      <c r="L14" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="D15" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="46">
+      <c r="G22" s="17">
         <v>5</v>
       </c>
-      <c r="F15" s="46">
-        <v>4</v>
-      </c>
-      <c r="G15" s="65">
-        <v>3</v>
-      </c>
-      <c r="H15" s="65">
-        <v>2</v>
-      </c>
-      <c r="I15" s="65">
-        <v>1</v>
-      </c>
-      <c r="J15" s="65">
-        <v>0</v>
-      </c>
-      <c r="K15" s="56">
-        <v>0</v>
-      </c>
-      <c r="L15" s="63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="61"/>
-      <c r="C16" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="64"/>
-    </row>
-    <row r="17" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D17" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="E17" s="46">
-        <v>15</v>
-      </c>
-      <c r="F17" s="46">
-        <v>15</v>
-      </c>
-      <c r="G17" s="65">
-        <v>12</v>
-      </c>
-      <c r="H17" s="65">
-        <v>10</v>
-      </c>
-      <c r="I17" s="65">
-        <v>8</v>
-      </c>
-      <c r="J17" s="65">
-        <v>7</v>
-      </c>
-      <c r="K17" s="56">
+      <c r="H22" s="17">
         <v>5</v>
       </c>
-      <c r="L17" s="63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
-      <c r="B18" s="61"/>
-      <c r="C18" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="64"/>
-    </row>
-    <row r="19" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="47"/>
-      <c r="C19" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E19" s="15">
-        <v>7</v>
-      </c>
-      <c r="F19" s="15">
-        <v>6</v>
-      </c>
-      <c r="G19" s="22">
-        <v>5</v>
-      </c>
-      <c r="H19" s="22">
-        <v>4</v>
-      </c>
-      <c r="I19" s="22">
-        <v>3</v>
-      </c>
-      <c r="J19" s="22">
-        <v>2</v>
-      </c>
-      <c r="K19" s="22">
-        <v>0</v>
-      </c>
-      <c r="L19" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
-      <c r="B20" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="17">
-        <v>25</v>
-      </c>
-      <c r="F20" s="17">
-        <v>23</v>
-      </c>
-      <c r="G20" s="19">
-        <v>20</v>
-      </c>
-      <c r="H20" s="19">
-        <v>18</v>
-      </c>
-      <c r="I20" s="19">
-        <v>17</v>
-      </c>
-      <c r="J20" s="19">
-        <v>12</v>
-      </c>
-      <c r="K20" s="19">
-        <v>8</v>
-      </c>
-      <c r="L20" s="36">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E21" s="17">
-        <v>5</v>
-      </c>
-      <c r="F21" s="17">
-        <v>5</v>
-      </c>
-      <c r="G21" s="19">
-        <v>5</v>
-      </c>
-      <c r="H21" s="19">
-        <v>5</v>
-      </c>
-      <c r="I21" s="19">
-        <v>2</v>
-      </c>
-      <c r="J21" s="19">
-        <v>2</v>
-      </c>
-      <c r="K21" s="19">
-        <v>0</v>
-      </c>
-      <c r="L21" s="36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="17">
-        <v>5</v>
-      </c>
-      <c r="F22" s="17">
-        <v>5</v>
-      </c>
-      <c r="G22" s="19">
-        <v>5</v>
-      </c>
-      <c r="H22" s="19">
-        <v>5</v>
-      </c>
-      <c r="I22" s="19">
-        <v>0</v>
-      </c>
-      <c r="J22" s="19">
-        <v>0</v>
-      </c>
-      <c r="K22" s="19">
-        <v>0</v>
-      </c>
-      <c r="L22" s="36">
+      <c r="I22" s="17">
+        <v>0</v>
+      </c>
+      <c r="J22" s="17">
+        <v>0</v>
+      </c>
+      <c r="K22" s="17">
+        <v>0</v>
+      </c>
+      <c r="L22" s="34">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
     <mergeCell ref="K15:K16"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F7:L7"/>
@@ -3864,14 +4234,6 @@
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="J15:J16"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3879,4 +4241,309 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D1BEA3-8F28-0B4B-9E6B-1A4498029C05}">
+  <dimension ref="A1:M18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="10.83203125" style="64"/>
+    <col min="3" max="3" width="23.5" style="64" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" style="64" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="64"/>
+    <col min="6" max="6" width="21.1640625" style="64" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="64"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="84" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
+    </row>
+    <row r="5" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="81" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="79"/>
+    </row>
+    <row r="7" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="77" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" s="77" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="77">
+        <v>1</v>
+      </c>
+      <c r="H7" s="77">
+        <v>2</v>
+      </c>
+      <c r="I7" s="77">
+        <v>3</v>
+      </c>
+      <c r="J7" s="77">
+        <v>4</v>
+      </c>
+      <c r="K7" s="77">
+        <v>5</v>
+      </c>
+      <c r="L7" s="77">
+        <v>6</v>
+      </c>
+      <c r="M7" s="76">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C8" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="74">
+        <v>10</v>
+      </c>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C9" s="73" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="E9" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="65">
+        <v>5</v>
+      </c>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="65"/>
+      <c r="M9" s="65"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C10" s="69"/>
+      <c r="D10" s="66" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="65">
+        <v>8</v>
+      </c>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C11" s="73" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="65">
+        <v>6</v>
+      </c>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="65"/>
+      <c r="K11" s="65"/>
+      <c r="L11" s="65"/>
+      <c r="M11" s="65"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C12" s="70"/>
+      <c r="D12" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="65">
+        <v>8</v>
+      </c>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="65"/>
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="65"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C13" s="70"/>
+      <c r="D13" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="65">
+        <v>6</v>
+      </c>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="65"/>
+      <c r="K13" s="65"/>
+      <c r="L13" s="65"/>
+      <c r="M13" s="65"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C14" s="70"/>
+      <c r="D14" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="65">
+        <v>2</v>
+      </c>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="67"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="67"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C15" s="70"/>
+      <c r="D15" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="65" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="65">
+        <v>10</v>
+      </c>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C16" s="70"/>
+      <c r="D16" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="E16" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="65">
+        <v>5</v>
+      </c>
+      <c r="G16" s="67"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="67"/>
+      <c r="J16" s="67"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C17" s="69"/>
+      <c r="D17" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="65">
+        <v>3</v>
+      </c>
+      <c r="G17" s="67"/>
+      <c r="H17" s="67"/>
+      <c r="I17" s="67"/>
+      <c r="J17" s="67"/>
+      <c r="K17" s="67"/>
+      <c r="L17" s="67"/>
+      <c r="M17" s="67"/>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C18" s="65" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="65">
+        <v>25</v>
+      </c>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
+      <c r="K18" s="65"/>
+      <c r="L18" s="65"/>
+      <c r="M18" s="65"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C11:C17"/>
+    <mergeCell ref="C9:C10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Backlog delayed update: end of Sprint 3, definition & progress of Sprint 4
</commit_message>
<xml_diff>
--- a/process/Project Backlog.xlsx
+++ b/process/Project Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardoperugini/Desktop/PPS-19-Primer/process/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62DAFBD-5DD5-5C4E-AEE7-8CBFDC235904}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1233B04B-EF49-2E49-B095-AEBD093788B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Riepilogo di esportazione" sheetId="1" r:id="rId1"/>
@@ -18,13 +18,14 @@
     <sheet name="1 Sprint Backlog" sheetId="3" r:id="rId3"/>
     <sheet name="2 Sprint Backlog" sheetId="4" r:id="rId4"/>
     <sheet name="3 Sprint Backlog" sheetId="5" r:id="rId5"/>
+    <sheet name="4 Sprint Backlog" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="119">
   <si>
     <t>Questo documento è stato esportato da Numbers. Tutte le tabelle sono state convertite in un foglio di lavoro di Excel. Tutti gli altri oggetti di ciascun foglio di Numbers sono stati collocati in fogli di lavoro separati. Nota che i calcoli delle formule potrebbero differire in Excel.</t>
   </si>
@@ -122,9 +123,6 @@
     <t>Utilizzo del paradigma funzionale per lo sviluppo dei test</t>
   </si>
   <si>
-    <t>[Opt] Gestione di un 'sense' base tra blob</t>
-  </si>
-  <si>
     <t>Definizione di un sistema base per facilitare le creature nella ricerca del cibo</t>
   </si>
   <si>
@@ -348,6 +346,42 @@
   </si>
   <si>
     <t>F/L</t>
+  </si>
+  <si>
+    <t>Aggiunta di strumenti per test Coverage</t>
+  </si>
+  <si>
+    <t>Aggiunta modifica geni alle creature</t>
+  </si>
+  <si>
+    <t>Rimozione di riferimenti di Model all'interno della View</t>
+  </si>
+  <si>
+    <t>Ulteriore Tuning dei parametri di simulazione</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conclusione report. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ulteriore suddivisione del simulatore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactoring dei test. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactoring dello stile. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inclusione di tool per la pulizia del codice. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suddivisione simulatore </t>
+  </si>
+  <si>
+    <t>Aggiunta geni al modello</t>
+  </si>
+  <si>
+    <t>[Abandoned] Gestione di un 'sense' base tra blob</t>
   </si>
 </sst>
 </file>
@@ -802,7 +836,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -958,38 +992,56 @@
     <xf numFmtId="49" fontId="4" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1007,19 +1059,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2239,11 +2288,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="61" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
+      <c r="B3" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
     </row>
     <row r="7" spans="2:4" ht="19" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
@@ -2274,7 +2323,7 @@
     </row>
     <row r="11" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -2285,12 +2334,12 @@
         <v>5</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -2301,7 +2350,7 @@
         <v>5</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2319,16 +2368,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="83" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="36.1640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="42.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67" style="5" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="5" customWidth="1"/>
     <col min="6" max="6" width="21.5" style="5" customWidth="1"/>
@@ -2337,12 +2386,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2380,13 +2429,13 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="73" t="s">
+      <c r="F4" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="75"/>
+      <c r="G4" s="80"/>
+      <c r="H4" s="80"/>
+      <c r="I4" s="80"/>
+      <c r="J4" s="81"/>
     </row>
     <row r="5" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
@@ -2418,137 +2467,147 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="53" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
-      <c r="B6" s="58">
+    <row r="6" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12"/>
+      <c r="B6" s="15">
         <v>1</v>
       </c>
-      <c r="C6" s="57" t="s">
-        <v>103</v>
-      </c>
-      <c r="D6" s="57" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6" s="58">
-        <v>10</v>
-      </c>
-      <c r="G6" s="58">
-        <v>10</v>
-      </c>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-    </row>
-    <row r="7" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="37">
+        <v>5</v>
+      </c>
+      <c r="F6" s="37">
+        <v>5</v>
+      </c>
+      <c r="G6" s="38">
+        <v>5</v>
+      </c>
+      <c r="H6" s="38">
+        <v>5</v>
+      </c>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
-      <c r="B7" s="65">
+      <c r="B7" s="73">
         <v>2</v>
       </c>
-      <c r="C7" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="56" t="s">
-        <v>105</v>
-      </c>
-      <c r="E7" s="68">
-        <v>5</v>
-      </c>
-      <c r="F7" s="68">
-        <v>5</v>
-      </c>
-      <c r="G7" s="63">
-        <v>5</v>
-      </c>
-      <c r="H7" s="63"/>
-      <c r="I7" s="63"/>
-      <c r="J7" s="63"/>
-    </row>
-    <row r="8" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C7" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="76">
+        <v>7</v>
+      </c>
+      <c r="F7" s="76">
+        <v>2</v>
+      </c>
+      <c r="G7" s="78">
+        <v>1</v>
+      </c>
+      <c r="H7" s="78">
+        <v>1</v>
+      </c>
+      <c r="I7" s="78"/>
+      <c r="J7" s="78"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="60" t="s">
-        <v>106</v>
-      </c>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+    </row>
+    <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="15">
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="37">
-        <v>17</v>
-      </c>
-      <c r="F9" s="37">
-        <v>17</v>
-      </c>
-      <c r="G9" s="38">
-        <v>17</v>
-      </c>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="38"/>
+        <v>12</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="35">
+        <v>20</v>
+      </c>
+      <c r="F9" s="35">
+        <v>20</v>
+      </c>
+      <c r="G9" s="36">
+        <v>2</v>
+      </c>
+      <c r="H9" s="36">
+        <v>2</v>
+      </c>
+      <c r="I9" s="36"/>
+      <c r="J9" s="36"/>
     </row>
     <row r="10" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="15">
         <v>4</v>
       </c>
-      <c r="C10" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="37">
-        <v>10</v>
-      </c>
-      <c r="F10" s="37">
-        <v>10</v>
-      </c>
-      <c r="G10" s="38">
-        <v>3</v>
-      </c>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
+      <c r="C10" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="35">
+        <v>11</v>
+      </c>
+      <c r="F10" s="35">
+        <v>11</v>
+      </c>
+      <c r="G10" s="36">
+        <v>2</v>
+      </c>
+      <c r="H10" s="36">
+        <v>2</v>
+      </c>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
     </row>
     <row r="11" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="15">
         <v>5</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>32</v>
+      <c r="C11" s="59" t="s">
+        <v>100</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E11" s="37">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F11" s="37">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G11" s="38">
-        <v>5</v>
-      </c>
-      <c r="H11" s="38"/>
+        <v>3</v>
+      </c>
+      <c r="H11" s="38">
+        <v>1</v>
+      </c>
       <c r="I11" s="38"/>
       <c r="J11" s="38"/>
     </row>
@@ -2558,271 +2617,289 @@
         <v>6</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="E12" s="37">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F12" s="37">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G12" s="38">
-        <v>5</v>
-      </c>
-      <c r="H12" s="38"/>
+        <v>1</v>
+      </c>
+      <c r="H12" s="38">
+        <v>1</v>
+      </c>
       <c r="I12" s="38"/>
       <c r="J12" s="38"/>
     </row>
     <row r="13" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
-      <c r="B13" s="15">
+      <c r="B13" s="73">
         <v>7</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="35">
-        <v>30</v>
-      </c>
-      <c r="F13" s="35">
-        <v>25</v>
-      </c>
-      <c r="G13" s="36">
-        <v>20</v>
-      </c>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
-    </row>
-    <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C13" s="75" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="76">
+        <v>8</v>
+      </c>
+      <c r="F13" s="76">
+        <v>8</v>
+      </c>
+      <c r="G13" s="78">
+        <v>1</v>
+      </c>
+      <c r="H13" s="78">
+        <v>1</v>
+      </c>
+      <c r="I13" s="78"/>
+      <c r="J13" s="78"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
-      <c r="B14" s="15">
-        <v>8</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="35">
-        <v>20</v>
-      </c>
-      <c r="F14" s="35">
-        <v>20</v>
-      </c>
-      <c r="G14" s="36">
-        <v>2</v>
-      </c>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
     </row>
     <row r="15" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="15">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D15" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="35">
+        <v>30</v>
+      </c>
+      <c r="F15" s="35">
+        <v>25</v>
+      </c>
+      <c r="G15" s="36">
         <v>20</v>
       </c>
-      <c r="E15" s="35">
-        <v>11</v>
-      </c>
-      <c r="F15" s="35">
-        <v>11</v>
-      </c>
-      <c r="G15" s="36">
-        <v>2</v>
-      </c>
-      <c r="H15" s="36"/>
+      <c r="H15" s="36">
+        <v>10</v>
+      </c>
       <c r="I15" s="36"/>
       <c r="J15" s="36"/>
     </row>
-    <row r="16" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="15">
+        <v>9</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="37">
         <v>10</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="37">
-        <v>7</v>
-      </c>
       <c r="F16" s="37">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G16" s="38">
+        <v>3</v>
+      </c>
+      <c r="H16" s="38">
         <v>1</v>
       </c>
-      <c r="H16" s="38"/>
       <c r="I16" s="38"/>
       <c r="J16" s="38"/>
     </row>
-    <row r="17" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
-      <c r="B17" s="72">
+    <row r="17" spans="1:10" s="53" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="52"/>
+      <c r="B17" s="58">
+        <v>10</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17" s="58">
+        <v>10</v>
+      </c>
+      <c r="G17" s="58">
+        <v>10</v>
+      </c>
+      <c r="H17" s="58">
+        <v>0</v>
+      </c>
+      <c r="I17" s="58"/>
+      <c r="J17" s="58"/>
+    </row>
+    <row r="18" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="12"/>
+      <c r="B18" s="85">
         <v>11</v>
       </c>
-      <c r="C17" s="71" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="70">
-        <v>8</v>
-      </c>
-      <c r="F17" s="70">
-        <v>8</v>
-      </c>
-      <c r="G17" s="69">
-        <v>1</v>
-      </c>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="64"/>
-      <c r="J18" s="64"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C18" s="86" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="56" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="87">
+        <v>5</v>
+      </c>
+      <c r="F18" s="87">
+        <v>5</v>
+      </c>
+      <c r="G18" s="84">
+        <v>5</v>
+      </c>
+      <c r="H18" s="84">
+        <v>0</v>
+      </c>
+      <c r="I18" s="84"/>
+      <c r="J18" s="84"/>
+    </row>
+    <row r="19" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
-      <c r="B19" s="72">
-        <v>12</v>
-      </c>
-      <c r="C19" s="71" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19" s="70">
-        <v>7</v>
-      </c>
-      <c r="F19" s="70">
-        <v>2</v>
-      </c>
-      <c r="G19" s="69">
-        <v>1</v>
-      </c>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="74"/>
+      <c r="D19" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="77"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="77"/>
     </row>
     <row r="20" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
-      <c r="B20" s="66"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="64"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
+      <c r="B20" s="15">
+        <v>12</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="37">
+        <v>17</v>
+      </c>
+      <c r="F20" s="37">
+        <v>17</v>
+      </c>
+      <c r="G20" s="38">
+        <v>17</v>
+      </c>
+      <c r="H20" s="38">
+        <v>0</v>
+      </c>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
     </row>
     <row r="21" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
-      <c r="B21" s="65">
+      <c r="B21" s="85">
         <v>13</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="86" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="68">
+      <c r="E21" s="87">
         <v>15</v>
       </c>
-      <c r="F21" s="68">
+      <c r="F21" s="87">
         <v>15</v>
       </c>
-      <c r="G21" s="63">
-        <v>0</v>
-      </c>
-      <c r="H21" s="63"/>
-      <c r="I21" s="63"/>
-      <c r="J21" s="63"/>
+      <c r="G21" s="84">
+        <v>0</v>
+      </c>
+      <c r="H21" s="84">
+        <v>0</v>
+      </c>
+      <c r="I21" s="84"/>
+      <c r="J21" s="84"/>
     </row>
     <row r="22" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
-      <c r="B22" s="66"/>
-      <c r="C22" s="66"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
       <c r="D22" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
-      <c r="I22" s="64"/>
-      <c r="J22" s="64"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="77"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="77"/>
+      <c r="I22" s="77"/>
+      <c r="J22" s="77"/>
     </row>
     <row r="23" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
-      <c r="B23" s="79">
+      <c r="B23" s="69">
         <v>14</v>
       </c>
-      <c r="C23" s="81" t="s">
+      <c r="C23" s="71" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="82">
-        <v>5</v>
-      </c>
-      <c r="F23" s="82">
-        <v>0</v>
-      </c>
-      <c r="G23" s="78">
-        <v>0</v>
-      </c>
-      <c r="H23" s="78"/>
-      <c r="I23" s="78"/>
-      <c r="J23" s="78"/>
+      <c r="E23" s="72">
+        <v>5</v>
+      </c>
+      <c r="F23" s="72">
+        <v>0</v>
+      </c>
+      <c r="G23" s="68">
+        <v>0</v>
+      </c>
+      <c r="H23" s="68">
+        <v>0</v>
+      </c>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
     </row>
     <row r="24" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
-      <c r="B24" s="80"/>
-      <c r="C24" s="80"/>
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
       <c r="D24" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
-      <c r="I24" s="78"/>
-      <c r="J24" s="78"/>
+        <v>37</v>
+      </c>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
     </row>
     <row r="25" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
@@ -2830,10 +2907,10 @@
         <v>15</v>
       </c>
       <c r="C25" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>39</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>40</v>
       </c>
       <c r="E25" s="35">
         <v>3</v>
@@ -2844,7 +2921,9 @@
       <c r="G25" s="36">
         <v>0</v>
       </c>
-      <c r="H25" s="36"/>
+      <c r="H25" s="36">
+        <v>0</v>
+      </c>
       <c r="I25" s="36"/>
       <c r="J25" s="36"/>
     </row>
@@ -2854,10 +2933,10 @@
         <v>16</v>
       </c>
       <c r="C26" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="14" t="s">
         <v>41</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="E26" s="35">
         <v>4</v>
@@ -2868,12 +2947,74 @@
       <c r="G26" s="36">
         <v>0</v>
       </c>
-      <c r="H26" s="36"/>
+      <c r="H26" s="36">
+        <v>0</v>
+      </c>
       <c r="I26" s="36"/>
       <c r="J26" s="36"/>
     </row>
+    <row r="27" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="12"/>
+      <c r="B27" s="15">
+        <v>17</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="37">
+        <v>5</v>
+      </c>
+      <c r="F27" s="37">
+        <v>5</v>
+      </c>
+      <c r="G27" s="38">
+        <v>5</v>
+      </c>
+      <c r="H27" s="38">
+        <v>5</v>
+      </c>
+      <c r="I27" s="38"/>
+      <c r="J27" s="38"/>
+    </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="H21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:J22"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="F7:F8"/>
     <mergeCell ref="H23:H24"/>
     <mergeCell ref="I23:I24"/>
     <mergeCell ref="J23:J24"/>
@@ -2882,40 +3023,6 @@
     <mergeCell ref="E23:E24"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="G23:G24"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="H21:H22"/>
-    <mergeCell ref="I21:I22"/>
-    <mergeCell ref="J21:J22"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G21:G22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -2945,12 +3052,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -3004,28 +3111,28 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="22"/>
-      <c r="F5" s="73" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="84"/>
+      <c r="F5" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="89"/>
     </row>
     <row r="6" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="D6" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="E6" s="23" t="s">
         <v>47</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>48</v>
       </c>
       <c r="F6" s="24">
         <v>1</v>
@@ -3048,14 +3155,14 @@
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
-      <c r="B7" s="86" t="s">
-        <v>36</v>
+      <c r="B7" s="91" t="s">
+        <v>35</v>
       </c>
       <c r="C7" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="26" t="s">
         <v>49</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>50</v>
       </c>
       <c r="E7" s="27">
         <v>7</v>
@@ -3081,12 +3188,12 @@
     </row>
     <row r="8" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
-      <c r="B8" s="85"/>
+      <c r="B8" s="90"/>
       <c r="C8" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8" s="13">
         <v>3</v>
@@ -3112,12 +3219,12 @@
     </row>
     <row r="9" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
-      <c r="B9" s="85"/>
+      <c r="B9" s="90"/>
       <c r="C9" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" s="13">
         <v>3</v>
@@ -3143,12 +3250,12 @@
     </row>
     <row r="10" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
-      <c r="B10" s="85"/>
+      <c r="B10" s="90"/>
       <c r="C10" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10" s="13">
         <v>7</v>
@@ -3174,12 +3281,12 @@
     </row>
     <row r="11" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
-      <c r="B11" s="66"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="13">
         <v>7</v>
@@ -3209,10 +3316,10 @@
         <v>24</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E12" s="13">
         <v>15</v>
@@ -3238,14 +3345,14 @@
     </row>
     <row r="13" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
-      <c r="B13" s="71" t="s">
-        <v>39</v>
+      <c r="B13" s="75" t="s">
+        <v>38</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E13" s="13">
         <v>2</v>
@@ -3271,12 +3378,12 @@
     </row>
     <row r="14" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
-      <c r="B14" s="85"/>
+      <c r="B14" s="90"/>
       <c r="C14" s="28" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="13">
         <v>3</v>
@@ -3302,12 +3409,12 @@
     </row>
     <row r="15" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
-      <c r="B15" s="85"/>
+      <c r="B15" s="90"/>
       <c r="C15" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E15" s="13">
         <v>2</v>
@@ -3333,12 +3440,12 @@
     </row>
     <row r="16" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
-      <c r="B16" s="85"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" s="13">
         <v>2</v>
@@ -3364,12 +3471,12 @@
     </row>
     <row r="17" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
-      <c r="B17" s="66"/>
+      <c r="B17" s="74"/>
       <c r="C17" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E17" s="13">
         <v>2</v>
@@ -3395,14 +3502,14 @@
     </row>
     <row r="18" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
-      <c r="B18" s="71" t="s">
-        <v>41</v>
+      <c r="B18" s="75" t="s">
+        <v>40</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E18" s="13">
         <v>3</v>
@@ -3428,12 +3535,12 @@
     </row>
     <row r="19" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
-      <c r="B19" s="66"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E19" s="13">
         <v>3</v>
@@ -3459,14 +3566,14 @@
     </row>
     <row r="20" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
-      <c r="B20" s="71" t="s">
+      <c r="B20" s="75" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" s="13">
         <v>4</v>
@@ -3492,12 +3599,12 @@
     </row>
     <row r="21" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
-      <c r="B21" s="85"/>
+      <c r="B21" s="90"/>
       <c r="C21" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>64</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>65</v>
       </c>
       <c r="E21" s="13">
         <v>5</v>
@@ -3523,12 +3630,12 @@
     </row>
     <row r="22" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
-      <c r="B22" s="85"/>
+      <c r="B22" s="90"/>
       <c r="C22" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="14" t="s">
         <v>66</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>67</v>
       </c>
       <c r="E22" s="13">
         <v>5</v>
@@ -3554,12 +3661,12 @@
     </row>
     <row r="23" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
-      <c r="B23" s="66"/>
+      <c r="B23" s="74"/>
       <c r="C23" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23" s="13">
         <v>5</v>
@@ -3620,12 +3727,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -3711,29 +3818,29 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="22"/>
-      <c r="F7" s="73" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="84"/>
+      <c r="F7" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="88"/>
+      <c r="H7" s="88"/>
+      <c r="I7" s="88"/>
+      <c r="J7" s="88"/>
+      <c r="K7" s="88"/>
+      <c r="L7" s="89"/>
     </row>
     <row r="8" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="D8" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="E8" s="23" t="s">
         <v>47</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>48</v>
       </c>
       <c r="F8" s="24">
         <v>1</v>
@@ -3759,14 +3866,14 @@
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="91" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>70</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>71</v>
       </c>
       <c r="E9" s="31">
         <v>5</v>
@@ -3795,12 +3902,12 @@
     </row>
     <row r="10" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
-      <c r="B10" s="85"/>
+      <c r="B10" s="90"/>
       <c r="C10" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" s="15">
         <v>10</v>
@@ -3829,12 +3936,12 @@
     </row>
     <row r="11" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
-      <c r="B11" s="85"/>
+      <c r="B11" s="90"/>
       <c r="C11" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" s="15">
         <v>12</v>
@@ -3863,12 +3970,12 @@
     </row>
     <row r="12" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
-      <c r="B12" s="66"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E12" s="13">
         <v>8</v>
@@ -3897,14 +4004,14 @@
     </row>
     <row r="13" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="75" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="13">
         <v>5</v>
@@ -3933,12 +4040,12 @@
     </row>
     <row r="14" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
-      <c r="B14" s="66"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E14" s="15">
         <v>10</v>
@@ -3967,114 +4074,114 @@
     </row>
     <row r="15" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
-      <c r="B15" s="71" t="s">
+      <c r="B15" s="75" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="72">
-        <v>5</v>
-      </c>
-      <c r="F15" s="72">
+        <v>76</v>
+      </c>
+      <c r="D15" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="73">
+        <v>5</v>
+      </c>
+      <c r="F15" s="73">
         <v>4</v>
       </c>
-      <c r="G15" s="89">
+      <c r="G15" s="94">
         <v>3</v>
       </c>
-      <c r="H15" s="89">
+      <c r="H15" s="94">
         <v>2</v>
       </c>
-      <c r="I15" s="89">
+      <c r="I15" s="94">
         <v>1</v>
       </c>
-      <c r="J15" s="89">
-        <v>0</v>
-      </c>
-      <c r="K15" s="80">
-        <v>0</v>
-      </c>
-      <c r="L15" s="87">
+      <c r="J15" s="94">
+        <v>0</v>
+      </c>
+      <c r="K15" s="70">
+        <v>0</v>
+      </c>
+      <c r="L15" s="92">
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
-      <c r="B16" s="85"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="66"/>
-      <c r="E16" s="66"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="66"/>
-      <c r="H16" s="66"/>
-      <c r="I16" s="66"/>
-      <c r="J16" s="66"/>
-      <c r="K16" s="80"/>
-      <c r="L16" s="88"/>
+        <v>77</v>
+      </c>
+      <c r="D16" s="74"/>
+      <c r="E16" s="74"/>
+      <c r="F16" s="74"/>
+      <c r="G16" s="74"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="93"/>
     </row>
     <row r="17" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
-      <c r="B17" s="85"/>
+      <c r="B17" s="90"/>
       <c r="C17" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="71" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="72">
+        <v>78</v>
+      </c>
+      <c r="D17" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="73">
         <v>15</v>
       </c>
-      <c r="F17" s="72">
+      <c r="F17" s="73">
         <v>15</v>
       </c>
-      <c r="G17" s="89">
+      <c r="G17" s="94">
         <v>12</v>
       </c>
-      <c r="H17" s="89">
+      <c r="H17" s="94">
         <v>10</v>
       </c>
-      <c r="I17" s="89">
+      <c r="I17" s="94">
         <v>8</v>
       </c>
-      <c r="J17" s="89">
+      <c r="J17" s="94">
         <v>7</v>
       </c>
-      <c r="K17" s="80">
-        <v>5</v>
-      </c>
-      <c r="L17" s="87">
+      <c r="K17" s="70">
+        <v>5</v>
+      </c>
+      <c r="L17" s="92">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
-      <c r="B18" s="85"/>
+      <c r="B18" s="90"/>
       <c r="C18" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="80"/>
-      <c r="L18" s="88"/>
+        <v>79</v>
+      </c>
+      <c r="D18" s="74"/>
+      <c r="E18" s="74"/>
+      <c r="F18" s="74"/>
+      <c r="G18" s="74"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="74"/>
+      <c r="K18" s="70"/>
+      <c r="L18" s="93"/>
     </row>
     <row r="19" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
-      <c r="B19" s="66"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E19" s="13">
         <v>7</v>
@@ -4107,10 +4214,10 @@
         <v>24</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" s="15">
         <v>25</v>
@@ -4140,13 +4247,13 @@
     <row r="21" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="14" t="s">
-        <v>83</v>
-      </c>
       <c r="D21" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" s="15">
         <v>5</v>
@@ -4176,13 +4283,13 @@
     <row r="22" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
       <c r="B22" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>85</v>
-      </c>
       <c r="D22" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E22" s="15">
         <v>5</v>
@@ -4211,6 +4318,14 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
     <mergeCell ref="K15:K16"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F7:L7"/>
@@ -4226,14 +4341,6 @@
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="J15:J16"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -4247,8 +4354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D1BEA3-8F28-0B4B-9E6B-1A4498029C05}">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView zoomScale="75" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4262,12 +4369,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="93" t="s">
+      <c r="A1" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
     </row>
     <row r="5" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4275,28 +4382,28 @@
       <c r="D6" s="51"/>
       <c r="E6" s="51"/>
       <c r="F6" s="51"/>
-      <c r="G6" s="90" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="91"/>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="92"/>
+      <c r="G6" s="95" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="96"/>
+      <c r="M6" s="97"/>
     </row>
     <row r="7" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C7" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="E7" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="49" t="s">
+      <c r="F7" s="49" t="s">
         <v>47</v>
-      </c>
-      <c r="F7" s="49" t="s">
-        <v>48</v>
       </c>
       <c r="G7" s="49">
         <v>1</v>
@@ -4322,13 +4429,13 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C8" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D8" s="47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" s="46">
         <v>10</v>
@@ -4348,18 +4455,22 @@
       <c r="K8" s="46">
         <v>0</v>
       </c>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
+      <c r="L8" s="61">
+        <v>0</v>
+      </c>
+      <c r="M8" s="61">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C9" s="95" t="s">
-        <v>97</v>
+      <c r="C9" s="100" t="s">
+        <v>96</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E9" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" s="40">
         <v>5</v>
@@ -4379,16 +4490,20 @@
       <c r="K9" s="40">
         <v>0</v>
       </c>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
+      <c r="L9" s="40">
+        <v>0</v>
+      </c>
+      <c r="M9" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C10" s="97"/>
+      <c r="C10" s="102"/>
       <c r="D10" s="41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E10" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F10" s="40">
         <v>8</v>
@@ -4408,18 +4523,22 @@
       <c r="K10" s="40">
         <v>8</v>
       </c>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
+      <c r="L10" s="40">
+        <v>8</v>
+      </c>
+      <c r="M10" s="40">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C11" s="95" t="s">
-        <v>94</v>
+      <c r="C11" s="100" t="s">
+        <v>93</v>
       </c>
       <c r="D11" s="45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E11" s="40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11" s="40">
         <v>6</v>
@@ -4439,16 +4558,20 @@
       <c r="K11" s="40">
         <v>0</v>
       </c>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
+      <c r="L11" s="40">
+        <v>0</v>
+      </c>
+      <c r="M11" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C12" s="96"/>
+      <c r="C12" s="101"/>
       <c r="D12" s="41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E12" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F12" s="40">
         <v>8</v>
@@ -4468,16 +4591,20 @@
       <c r="K12" s="40">
         <v>0</v>
       </c>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
+      <c r="L12" s="40">
+        <v>0</v>
+      </c>
+      <c r="M12" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C13" s="96"/>
+      <c r="C13" s="101"/>
       <c r="D13" s="41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E13" s="40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F13" s="40">
         <v>6</v>
@@ -4497,16 +4624,20 @@
       <c r="K13" s="40">
         <v>1</v>
       </c>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
+      <c r="L13" s="40">
+        <v>0</v>
+      </c>
+      <c r="M13" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C14" s="96"/>
+      <c r="C14" s="101"/>
       <c r="D14" s="41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E14" s="40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F14" s="40">
         <v>2</v>
@@ -4526,16 +4657,20 @@
       <c r="K14" s="40">
         <v>0</v>
       </c>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
+      <c r="L14" s="40">
+        <v>0</v>
+      </c>
+      <c r="M14" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C15" s="96"/>
+      <c r="C15" s="101"/>
       <c r="D15" s="44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F15" s="40">
         <v>10</v>
@@ -4555,16 +4690,20 @@
       <c r="K15" s="40">
         <v>0</v>
       </c>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
+      <c r="L15" s="40">
+        <v>0</v>
+      </c>
+      <c r="M15" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C16" s="96"/>
+      <c r="C16" s="101"/>
       <c r="D16" s="42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F16" s="40">
         <v>5</v>
@@ -4584,16 +4723,20 @@
       <c r="K16" s="40">
         <v>0</v>
       </c>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
+      <c r="L16" s="40">
+        <v>0</v>
+      </c>
+      <c r="M16" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="C17" s="97"/>
+      <c r="C17" s="102"/>
       <c r="D17" s="43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E17" s="40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F17" s="40">
         <v>3</v>
@@ -4613,18 +4756,22 @@
       <c r="K17" s="40">
         <v>3</v>
       </c>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
+      <c r="L17" s="40">
+        <v>3</v>
+      </c>
+      <c r="M17" s="40">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" s="40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E18" s="40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F18" s="40">
         <v>25</v>
@@ -4644,8 +4791,12 @@
       <c r="K18" s="40">
         <v>10</v>
       </c>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
+      <c r="L18" s="40">
+        <v>8</v>
+      </c>
+      <c r="M18" s="40">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4656,4 +4807,450 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CA0273-367C-3F42-94C6-B2C3E06A7BA4}">
+  <dimension ref="A1:M16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="98" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="39"/>
+    </row>
+    <row r="5" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="39"/>
+    </row>
+    <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+      <c r="E6" s="51"/>
+      <c r="F6" s="51"/>
+      <c r="G6" s="95" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="96"/>
+      <c r="M6" s="97"/>
+    </row>
+    <row r="7" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="63">
+        <v>1</v>
+      </c>
+      <c r="H7" s="63">
+        <v>2</v>
+      </c>
+      <c r="I7" s="63">
+        <v>3</v>
+      </c>
+      <c r="J7" s="63">
+        <v>4</v>
+      </c>
+      <c r="K7" s="63">
+        <v>5</v>
+      </c>
+      <c r="L7" s="63">
+        <v>6</v>
+      </c>
+      <c r="M7" s="64">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="65" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="65">
+        <v>1</v>
+      </c>
+      <c r="G8" s="65">
+        <v>1</v>
+      </c>
+      <c r="H8" s="65">
+        <v>1</v>
+      </c>
+      <c r="I8" s="65">
+        <v>0</v>
+      </c>
+      <c r="J8" s="65">
+        <v>0</v>
+      </c>
+      <c r="K8" s="65">
+        <v>0</v>
+      </c>
+      <c r="L8" s="65"/>
+      <c r="M8" s="65"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="40">
+        <v>5</v>
+      </c>
+      <c r="G9" s="40">
+        <v>5</v>
+      </c>
+      <c r="H9" s="40">
+        <v>5</v>
+      </c>
+      <c r="I9" s="40">
+        <v>4</v>
+      </c>
+      <c r="J9" s="40">
+        <v>0</v>
+      </c>
+      <c r="K9" s="40">
+        <v>0</v>
+      </c>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="65" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="40">
+        <v>5</v>
+      </c>
+      <c r="G10" s="40">
+        <v>5</v>
+      </c>
+      <c r="H10" s="40">
+        <v>4</v>
+      </c>
+      <c r="I10" s="40">
+        <v>2</v>
+      </c>
+      <c r="J10" s="40">
+        <v>1</v>
+      </c>
+      <c r="K10" s="40">
+        <v>0</v>
+      </c>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="100" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="40">
+        <v>5</v>
+      </c>
+      <c r="G11" s="40">
+        <v>5</v>
+      </c>
+      <c r="H11" s="40">
+        <v>0</v>
+      </c>
+      <c r="I11" s="40">
+        <v>0</v>
+      </c>
+      <c r="J11" s="40">
+        <v>0</v>
+      </c>
+      <c r="K11" s="40">
+        <v>0</v>
+      </c>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="41" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="40">
+        <v>5</v>
+      </c>
+      <c r="G12" s="40">
+        <v>5</v>
+      </c>
+      <c r="H12" s="40">
+        <v>5</v>
+      </c>
+      <c r="I12" s="40">
+        <v>5</v>
+      </c>
+      <c r="J12" s="40">
+        <v>5</v>
+      </c>
+      <c r="K12" s="40">
+        <v>5</v>
+      </c>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="101"/>
+      <c r="D13" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="40">
+        <v>2</v>
+      </c>
+      <c r="G13" s="40">
+        <v>2</v>
+      </c>
+      <c r="H13" s="40">
+        <v>2</v>
+      </c>
+      <c r="I13" s="40">
+        <v>2</v>
+      </c>
+      <c r="J13" s="40">
+        <v>2</v>
+      </c>
+      <c r="K13" s="40">
+        <v>1</v>
+      </c>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="39"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="40">
+        <v>3</v>
+      </c>
+      <c r="G14" s="40">
+        <v>3</v>
+      </c>
+      <c r="H14" s="40">
+        <v>3</v>
+      </c>
+      <c r="I14" s="40">
+        <v>3</v>
+      </c>
+      <c r="J14" s="40">
+        <v>3</v>
+      </c>
+      <c r="K14" s="40">
+        <v>3</v>
+      </c>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="39"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="102"/>
+      <c r="D15" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="40">
+        <v>3</v>
+      </c>
+      <c r="G15" s="40">
+        <v>3</v>
+      </c>
+      <c r="H15" s="40">
+        <v>3</v>
+      </c>
+      <c r="I15" s="40">
+        <v>3</v>
+      </c>
+      <c r="J15" s="40">
+        <v>3</v>
+      </c>
+      <c r="K15" s="40">
+        <v>3</v>
+      </c>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="39"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="40" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="40">
+        <v>15</v>
+      </c>
+      <c r="G16" s="40">
+        <v>15</v>
+      </c>
+      <c r="H16" s="40">
+        <v>13</v>
+      </c>
+      <c r="I16" s="40">
+        <v>10</v>
+      </c>
+      <c r="J16" s="40">
+        <v>8</v>
+      </c>
+      <c r="K16" s="40">
+        <v>7</v>
+      </c>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="C11:C15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Backlog Updated - End of Sprint 4 + minor changes
</commit_message>
<xml_diff>
--- a/process/Project Backlog.xlsx
+++ b/process/Project Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardoperugini/Desktop/PPS-19-Primer/process/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1233B04B-EF49-2E49-B095-AEBD093788B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969E95F6-3940-2F47-BE95-A8397D6375CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16780" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16760" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Riepilogo di esportazione" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -444,6 +444,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="13"/>
         <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -836,7 +842,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1011,37 +1017,31 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1059,16 +1059,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1114,6 +1120,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2370,8 +2397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="83" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2386,12 +2413,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -2429,13 +2456,13 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="79" t="s">
+      <c r="F4" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="81"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
+      <c r="J4" s="79"/>
     </row>
     <row r="5" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
@@ -2490,15 +2517,17 @@
       <c r="H6" s="38">
         <v>5</v>
       </c>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
+      <c r="I6" s="38">
+        <v>0</v>
+      </c>
+      <c r="J6" s="103"/>
     </row>
     <row r="7" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
-      <c r="B7" s="73">
+      <c r="B7" s="75">
         <v>2</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="74" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="18" t="s">
@@ -2510,28 +2539,30 @@
       <c r="F7" s="76">
         <v>2</v>
       </c>
-      <c r="G7" s="78">
+      <c r="G7" s="82">
         <v>1</v>
       </c>
-      <c r="H7" s="78">
+      <c r="H7" s="82">
         <v>1</v>
       </c>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78"/>
+      <c r="I7" s="82">
+        <v>0</v>
+      </c>
+      <c r="J7" s="104"/>
     </row>
     <row r="8" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
       <c r="D8" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="77"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="105"/>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
@@ -2556,8 +2587,10 @@
       <c r="H9" s="36">
         <v>2</v>
       </c>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
+      <c r="I9" s="36">
+        <v>0</v>
+      </c>
+      <c r="J9" s="106"/>
     </row>
     <row r="10" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
@@ -2582,8 +2615,10 @@
       <c r="H10" s="36">
         <v>2</v>
       </c>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="I10" s="36">
+        <v>0</v>
+      </c>
+      <c r="J10" s="106"/>
     </row>
     <row r="11" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
@@ -2608,8 +2643,10 @@
       <c r="H11" s="38">
         <v>1</v>
       </c>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
+      <c r="I11" s="38">
+        <v>0</v>
+      </c>
+      <c r="J11" s="103"/>
     </row>
     <row r="12" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
@@ -2634,15 +2671,17 @@
       <c r="H12" s="38">
         <v>1</v>
       </c>
-      <c r="I12" s="38"/>
-      <c r="J12" s="38"/>
+      <c r="I12" s="38">
+        <v>0</v>
+      </c>
+      <c r="J12" s="103"/>
     </row>
     <row r="13" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
-      <c r="B13" s="73">
+      <c r="B13" s="75">
         <v>7</v>
       </c>
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="74" t="s">
         <v>16</v>
       </c>
       <c r="D13" s="18" t="s">
@@ -2654,28 +2693,30 @@
       <c r="F13" s="76">
         <v>8</v>
       </c>
-      <c r="G13" s="78">
+      <c r="G13" s="82">
         <v>1</v>
       </c>
-      <c r="H13" s="78">
+      <c r="H13" s="82">
         <v>1</v>
       </c>
-      <c r="I13" s="78"/>
-      <c r="J13" s="78"/>
+      <c r="I13" s="82">
+        <v>0</v>
+      </c>
+      <c r="J13" s="104"/>
     </row>
     <row r="14" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="71"/>
       <c r="D14" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="77"/>
-      <c r="F14" s="77"/>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="77"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="105"/>
     </row>
     <row r="15" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
@@ -2700,8 +2741,10 @@
       <c r="H15" s="36">
         <v>10</v>
       </c>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
+      <c r="I15" s="36">
+        <v>0</v>
+      </c>
+      <c r="J15" s="106"/>
     </row>
     <row r="16" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
@@ -2726,8 +2769,10 @@
       <c r="H16" s="38">
         <v>1</v>
       </c>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
+      <c r="I16" s="38">
+        <v>0</v>
+      </c>
+      <c r="J16" s="103"/>
     </row>
     <row r="17" spans="1:10" s="53" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="52"/>
@@ -2752,48 +2797,52 @@
       <c r="H17" s="58">
         <v>0</v>
       </c>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
+      <c r="I17" s="58">
+        <v>0</v>
+      </c>
+      <c r="J17" s="107"/>
     </row>
     <row r="18" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
-      <c r="B18" s="85">
+      <c r="B18" s="70">
         <v>11</v>
       </c>
-      <c r="C18" s="86" t="s">
+      <c r="C18" s="72" t="s">
         <v>99</v>
       </c>
       <c r="D18" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="87">
-        <v>5</v>
-      </c>
-      <c r="F18" s="87">
-        <v>5</v>
-      </c>
-      <c r="G18" s="84">
-        <v>5</v>
-      </c>
-      <c r="H18" s="84">
-        <v>0</v>
-      </c>
-      <c r="I18" s="84"/>
-      <c r="J18" s="84"/>
+      <c r="E18" s="73">
+        <v>5</v>
+      </c>
+      <c r="F18" s="73">
+        <v>5</v>
+      </c>
+      <c r="G18" s="68">
+        <v>5</v>
+      </c>
+      <c r="H18" s="68">
+        <v>0</v>
+      </c>
+      <c r="I18" s="68">
+        <v>0</v>
+      </c>
+      <c r="J18" s="108"/>
     </row>
     <row r="19" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
-      <c r="B19" s="74"/>
-      <c r="C19" s="74"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
       <c r="D19" s="60" t="s">
         <v>105</v>
       </c>
-      <c r="E19" s="77"/>
-      <c r="F19" s="77"/>
-      <c r="G19" s="77"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="77"/>
-      <c r="J19" s="77"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="105"/>
     </row>
     <row r="20" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
@@ -2818,88 +2867,94 @@
       <c r="H20" s="38">
         <v>0</v>
       </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="I20" s="38">
+        <v>0</v>
+      </c>
+      <c r="J20" s="103"/>
     </row>
     <row r="21" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
-      <c r="B21" s="85">
+      <c r="B21" s="70">
         <v>13</v>
       </c>
-      <c r="C21" s="86" t="s">
+      <c r="C21" s="72" t="s">
         <v>21</v>
       </c>
       <c r="D21" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="87">
+      <c r="E21" s="73">
         <v>15</v>
       </c>
-      <c r="F21" s="87">
+      <c r="F21" s="73">
         <v>15</v>
       </c>
-      <c r="G21" s="84">
-        <v>0</v>
-      </c>
-      <c r="H21" s="84">
-        <v>0</v>
-      </c>
-      <c r="I21" s="84"/>
-      <c r="J21" s="84"/>
+      <c r="G21" s="68">
+        <v>0</v>
+      </c>
+      <c r="H21" s="68">
+        <v>0</v>
+      </c>
+      <c r="I21" s="68">
+        <v>0</v>
+      </c>
+      <c r="J21" s="108"/>
     </row>
     <row r="22" spans="1:10" s="29" customFormat="1" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="12"/>
-      <c r="B22" s="74"/>
-      <c r="C22" s="74"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
       <c r="D22" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="77"/>
-      <c r="F22" s="77"/>
-      <c r="G22" s="77"/>
-      <c r="H22" s="77"/>
-      <c r="I22" s="77"/>
-      <c r="J22" s="77"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="105"/>
     </row>
     <row r="23" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
-      <c r="B23" s="69">
+      <c r="B23" s="84">
         <v>14</v>
       </c>
-      <c r="C23" s="71" t="s">
+      <c r="C23" s="86" t="s">
         <v>35</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="72">
-        <v>5</v>
-      </c>
-      <c r="F23" s="72">
-        <v>0</v>
-      </c>
-      <c r="G23" s="68">
-        <v>0</v>
-      </c>
-      <c r="H23" s="68">
-        <v>0</v>
-      </c>
-      <c r="I23" s="68"/>
-      <c r="J23" s="68"/>
+      <c r="E23" s="87">
+        <v>5</v>
+      </c>
+      <c r="F23" s="87">
+        <v>0</v>
+      </c>
+      <c r="G23" s="83">
+        <v>0</v>
+      </c>
+      <c r="H23" s="83">
+        <v>0</v>
+      </c>
+      <c r="I23" s="83">
+        <v>0</v>
+      </c>
+      <c r="J23" s="109"/>
     </row>
     <row r="24" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
-      <c r="B24" s="70"/>
-      <c r="C24" s="70"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="68"/>
+      <c r="E24" s="83"/>
+      <c r="F24" s="83"/>
+      <c r="G24" s="83"/>
+      <c r="H24" s="83"/>
+      <c r="I24" s="83"/>
+      <c r="J24" s="109"/>
     </row>
     <row r="25" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="12"/>
@@ -2924,8 +2979,10 @@
       <c r="H25" s="36">
         <v>0</v>
       </c>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
+      <c r="I25" s="36">
+        <v>0</v>
+      </c>
+      <c r="J25" s="106"/>
     </row>
     <row r="26" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="12"/>
@@ -2950,8 +3007,10 @@
       <c r="H26" s="36">
         <v>0</v>
       </c>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
+      <c r="I26" s="36">
+        <v>0</v>
+      </c>
+      <c r="J26" s="106"/>
     </row>
     <row r="27" spans="1:10" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12"/>
@@ -2976,11 +3035,39 @@
       <c r="H27" s="38">
         <v>5</v>
       </c>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
+      <c r="I27" s="38">
+        <v>5</v>
+      </c>
+      <c r="J27" s="103"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G23:G24"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="H7:H8"/>
     <mergeCell ref="H21:H22"/>
     <mergeCell ref="I21:I22"/>
     <mergeCell ref="J21:J22"/>
@@ -2997,32 +3084,6 @@
     <mergeCell ref="E21:E22"/>
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="G21:G22"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="H23:H24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="G23:G24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3052,12 +3113,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -3111,7 +3172,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="22"/>
-      <c r="F5" s="79" t="s">
+      <c r="F5" s="77" t="s">
         <v>43</v>
       </c>
       <c r="G5" s="88"/>
@@ -3281,7 +3342,7 @@
     </row>
     <row r="11" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
-      <c r="B11" s="74"/>
+      <c r="B11" s="71"/>
       <c r="C11" s="28" t="s">
         <v>53</v>
       </c>
@@ -3345,7 +3406,7 @@
     </row>
     <row r="13" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="74" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="28" t="s">
@@ -3471,7 +3532,7 @@
     </row>
     <row r="17" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
-      <c r="B17" s="74"/>
+      <c r="B17" s="71"/>
       <c r="C17" s="28" t="s">
         <v>59</v>
       </c>
@@ -3502,7 +3563,7 @@
     </row>
     <row r="18" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="74" t="s">
         <v>40</v>
       </c>
       <c r="C18" s="28" t="s">
@@ -3535,7 +3596,7 @@
     </row>
     <row r="19" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
-      <c r="B19" s="74"/>
+      <c r="B19" s="71"/>
       <c r="C19" s="28" t="s">
         <v>61</v>
       </c>
@@ -3566,7 +3627,7 @@
     </row>
     <row r="20" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="74" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="28" t="s">
@@ -3661,7 +3722,7 @@
     </row>
     <row r="23" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="12"/>
-      <c r="B23" s="74"/>
+      <c r="B23" s="71"/>
       <c r="C23" s="28" t="s">
         <v>67</v>
       </c>
@@ -3727,12 +3788,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -3818,7 +3879,7 @@
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="22"/>
-      <c r="F7" s="79" t="s">
+      <c r="F7" s="77" t="s">
         <v>43</v>
       </c>
       <c r="G7" s="88"/>
@@ -3970,7 +4031,7 @@
     </row>
     <row r="12" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
-      <c r="B12" s="74"/>
+      <c r="B12" s="71"/>
       <c r="C12" s="16" t="s">
         <v>73</v>
       </c>
@@ -4004,7 +4065,7 @@
     </row>
     <row r="13" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12"/>
-      <c r="B13" s="75" t="s">
+      <c r="B13" s="74" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -4040,7 +4101,7 @@
     </row>
     <row r="14" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12"/>
-      <c r="B14" s="74"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="16" t="s">
         <v>75</v>
       </c>
@@ -4074,19 +4135,19 @@
     </row>
     <row r="15" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="74" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="D15" s="75" t="s">
+      <c r="D15" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="E15" s="73">
-        <v>5</v>
-      </c>
-      <c r="F15" s="73">
+      <c r="E15" s="75">
+        <v>5</v>
+      </c>
+      <c r="F15" s="75">
         <v>4</v>
       </c>
       <c r="G15" s="94">
@@ -4101,7 +4162,7 @@
       <c r="J15" s="94">
         <v>0</v>
       </c>
-      <c r="K15" s="70">
+      <c r="K15" s="85">
         <v>0</v>
       </c>
       <c r="L15" s="92">
@@ -4114,14 +4175,14 @@
       <c r="C16" s="19" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="74"/>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="74"/>
-      <c r="J16" s="74"/>
-      <c r="K16" s="70"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
+      <c r="G16" s="71"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="85"/>
       <c r="L16" s="93"/>
     </row>
     <row r="17" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4130,13 +4191,13 @@
       <c r="C17" s="18" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="75" t="s">
+      <c r="D17" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="E17" s="73">
+      <c r="E17" s="75">
         <v>15</v>
       </c>
-      <c r="F17" s="73">
+      <c r="F17" s="75">
         <v>15</v>
       </c>
       <c r="G17" s="94">
@@ -4151,7 +4212,7 @@
       <c r="J17" s="94">
         <v>7</v>
       </c>
-      <c r="K17" s="70">
+      <c r="K17" s="85">
         <v>5</v>
       </c>
       <c r="L17" s="92">
@@ -4164,19 +4225,19 @@
       <c r="C18" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="70"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="71"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="71"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="85"/>
       <c r="L18" s="93"/>
     </row>
     <row r="19" spans="1:12" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
-      <c r="B19" s="74"/>
+      <c r="B19" s="71"/>
       <c r="C19" s="14" t="s">
         <v>80</v>
       </c>
@@ -4318,14 +4379,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
     <mergeCell ref="K15:K16"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F7:L7"/>
@@ -4341,6 +4394,14 @@
     <mergeCell ref="H15:H16"/>
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="J15:J16"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -4813,8 +4874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CA0273-367C-3F42-94C6-B2C3E06A7BA4}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4986,8 +5047,12 @@
       <c r="K8" s="65">
         <v>0</v>
       </c>
-      <c r="L8" s="65"/>
-      <c r="M8" s="65"/>
+      <c r="L8" s="65">
+        <v>0</v>
+      </c>
+      <c r="M8" s="65">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="39"/>
@@ -5019,8 +5084,12 @@
       <c r="K9" s="40">
         <v>0</v>
       </c>
-      <c r="L9" s="40"/>
-      <c r="M9" s="40"/>
+      <c r="L9" s="40">
+        <v>0</v>
+      </c>
+      <c r="M9" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="39"/>
@@ -5052,8 +5121,12 @@
       <c r="K10" s="40">
         <v>0</v>
       </c>
-      <c r="L10" s="40"/>
-      <c r="M10" s="40"/>
+      <c r="L10" s="40">
+        <v>0</v>
+      </c>
+      <c r="M10" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="39"/>
@@ -5085,8 +5158,12 @@
       <c r="K11" s="40">
         <v>0</v>
       </c>
-      <c r="L11" s="40"/>
-      <c r="M11" s="40"/>
+      <c r="L11" s="40">
+        <v>0</v>
+      </c>
+      <c r="M11" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="39"/>
@@ -5116,8 +5193,12 @@
       <c r="K12" s="40">
         <v>5</v>
       </c>
-      <c r="L12" s="40"/>
-      <c r="M12" s="40"/>
+      <c r="L12" s="40">
+        <v>0</v>
+      </c>
+      <c r="M12" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="39"/>
@@ -5147,8 +5228,12 @@
       <c r="K13" s="40">
         <v>1</v>
       </c>
-      <c r="L13" s="40"/>
-      <c r="M13" s="40"/>
+      <c r="L13" s="40">
+        <v>0</v>
+      </c>
+      <c r="M13" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="39"/>
@@ -5178,8 +5263,12 @@
       <c r="K14" s="40">
         <v>3</v>
       </c>
-      <c r="L14" s="40"/>
-      <c r="M14" s="40"/>
+      <c r="L14" s="40">
+        <v>0</v>
+      </c>
+      <c r="M14" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="39"/>
@@ -5209,8 +5298,12 @@
       <c r="K15" s="40">
         <v>3</v>
       </c>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
+      <c r="L15" s="40">
+        <v>0</v>
+      </c>
+      <c r="M15" s="40">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="39"/>
@@ -5242,8 +5335,12 @@
       <c r="K16" s="40">
         <v>7</v>
       </c>
-      <c r="L16" s="40"/>
-      <c r="M16" s="40"/>
+      <c r="L16" s="40">
+        <v>3</v>
+      </c>
+      <c r="M16" s="40">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>